<commit_message>
Update dependencies and data sources
</commit_message>
<xml_diff>
--- a/data/usstations.xlsx
+++ b/data/usstations.xlsx
@@ -16,10 +16,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
-    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
-  </numFmts>
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -58,12 +55,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -518,11 +514,11 @@
           <t>Nawiliwili, HI</t>
         </is>
       </c>
-      <c r="C2" s="2" t="n">
-        <v>20090</v>
-      </c>
-      <c r="D2" s="2" t="n">
-        <v>44927</v>
+      <c r="C2" t="n">
+        <v>1955</v>
+      </c>
+      <c r="D2" t="n">
+        <v>2023</v>
       </c>
       <c r="E2" t="n">
         <v>69</v>
@@ -568,11 +564,11 @@
           <t>Honolulu, HI</t>
         </is>
       </c>
-      <c r="C3" s="2" t="n">
-        <v>1828</v>
-      </c>
-      <c r="D3" s="2" t="n">
-        <v>44927</v>
+      <c r="C3" t="n">
+        <v>1905</v>
+      </c>
+      <c r="D3" t="n">
+        <v>2023</v>
       </c>
       <c r="E3" t="n">
         <v>119</v>
@@ -618,11 +614,11 @@
           <t>Mokuoloe, HI</t>
         </is>
       </c>
-      <c r="C4" s="2" t="n">
-        <v>20821</v>
-      </c>
-      <c r="D4" s="2" t="n">
-        <v>44927</v>
+      <c r="C4" t="n">
+        <v>1957</v>
+      </c>
+      <c r="D4" t="n">
+        <v>2023</v>
       </c>
       <c r="E4" t="n">
         <v>67</v>
@@ -668,11 +664,11 @@
           <t>Kahului, HI</t>
         </is>
       </c>
-      <c r="C5" s="2" t="n">
-        <v>17168</v>
-      </c>
-      <c r="D5" s="2" t="n">
-        <v>44927</v>
+      <c r="C5" t="n">
+        <v>1947</v>
+      </c>
+      <c r="D5" t="n">
+        <v>2023</v>
       </c>
       <c r="E5" t="n">
         <v>77</v>
@@ -718,11 +714,11 @@
           <t>Kawaihae, HI</t>
         </is>
       </c>
-      <c r="C6" s="2" t="n">
-        <v>32143</v>
-      </c>
-      <c r="D6" s="2" t="n">
-        <v>44927</v>
+      <c r="C6" t="n">
+        <v>1988</v>
+      </c>
+      <c r="D6" t="n">
+        <v>2023</v>
       </c>
       <c r="E6" t="n">
         <v>36</v>
@@ -768,11 +764,11 @@
           <t>Hilo, HI</t>
         </is>
       </c>
-      <c r="C7" s="2" t="n">
-        <v>9863</v>
-      </c>
-      <c r="D7" s="2" t="n">
-        <v>44927</v>
+      <c r="C7" t="n">
+        <v>1927</v>
+      </c>
+      <c r="D7" t="n">
+        <v>2023</v>
       </c>
       <c r="E7" t="n">
         <v>97</v>
@@ -818,11 +814,11 @@
           <t>Midway Atoll, Unknown</t>
         </is>
       </c>
-      <c r="C8" s="2" t="n">
-        <v>17168</v>
-      </c>
-      <c r="D8" s="2" t="n">
-        <v>44927</v>
+      <c r="C8" t="n">
+        <v>1947</v>
+      </c>
+      <c r="D8" t="n">
+        <v>2023</v>
       </c>
       <c r="E8" t="n">
         <v>77</v>
@@ -868,11 +864,11 @@
           <t>Apra Harbor, Guam</t>
         </is>
       </c>
-      <c r="C9" s="2" t="n">
-        <v>33970</v>
-      </c>
-      <c r="D9" s="2" t="n">
-        <v>44927</v>
+      <c r="C9" t="n">
+        <v>1993</v>
+      </c>
+      <c r="D9" t="n">
+        <v>2023</v>
       </c>
       <c r="E9" t="n">
         <v>31</v>
@@ -918,11 +914,11 @@
           <t>Pago Pago, American Samoa</t>
         </is>
       </c>
-      <c r="C10" s="2" t="n">
-        <v>17533</v>
-      </c>
-      <c r="D10" s="2" t="n">
-        <v>39814</v>
+      <c r="C10" t="n">
+        <v>1948</v>
+      </c>
+      <c r="D10" t="n">
+        <v>2009</v>
       </c>
       <c r="E10" t="n">
         <v>62</v>
@@ -968,11 +964,11 @@
           <t>Kwajalein, Marshall Islands</t>
         </is>
       </c>
-      <c r="C11" s="2" t="n">
-        <v>16803</v>
-      </c>
-      <c r="D11" s="2" t="n">
-        <v>44927</v>
+      <c r="C11" t="n">
+        <v>1946</v>
+      </c>
+      <c r="D11" t="n">
+        <v>2023</v>
       </c>
       <c r="E11" t="n">
         <v>78</v>
@@ -1018,11 +1014,11 @@
           <t>Wake Island, Pacific Ocean</t>
         </is>
       </c>
-      <c r="C12" s="2" t="n">
-        <v>18264</v>
-      </c>
-      <c r="D12" s="2" t="n">
-        <v>44927</v>
+      <c r="C12" t="n">
+        <v>1950</v>
+      </c>
+      <c r="D12" t="n">
+        <v>2023</v>
       </c>
       <c r="E12" t="n">
         <v>74</v>
@@ -1068,11 +1064,11 @@
           <t>Biological Station, Bermuda</t>
         </is>
       </c>
-      <c r="C13" s="2" t="n">
-        <v>11689</v>
-      </c>
-      <c r="D13" s="2" t="n">
-        <v>44927</v>
+      <c r="C13" t="n">
+        <v>1932</v>
+      </c>
+      <c r="D13" t="n">
+        <v>2023</v>
       </c>
       <c r="E13" t="n">
         <v>92</v>
@@ -1118,11 +1114,11 @@
           <t>St. Georges, Bermuda</t>
         </is>
       </c>
-      <c r="C14" s="2" t="n">
-        <v>11689</v>
-      </c>
-      <c r="D14" s="2" t="n">
-        <v>43466</v>
+      <c r="C14" t="n">
+        <v>1932</v>
+      </c>
+      <c r="D14" t="n">
+        <v>2019</v>
       </c>
       <c r="E14" t="n">
         <v>88</v>
@@ -1168,11 +1164,11 @@
           <t>Eastport, ME</t>
         </is>
       </c>
-      <c r="C15" s="2" t="n">
-        <v>10594</v>
-      </c>
-      <c r="D15" s="2" t="n">
-        <v>44927</v>
+      <c r="C15" t="n">
+        <v>1929</v>
+      </c>
+      <c r="D15" t="n">
+        <v>2023</v>
       </c>
       <c r="E15" t="n">
         <v>95</v>
@@ -1218,11 +1214,11 @@
           <t>Cutler, ME</t>
         </is>
       </c>
-      <c r="C16" s="2" t="n">
-        <v>28856</v>
-      </c>
-      <c r="D16" s="2" t="n">
-        <v>40179</v>
+      <c r="C16" t="n">
+        <v>1979</v>
+      </c>
+      <c r="D16" t="n">
+        <v>2010</v>
       </c>
       <c r="E16" t="n">
         <v>32</v>
@@ -1268,11 +1264,11 @@
           <t>Bar Harbor, ME</t>
         </is>
       </c>
-      <c r="C17" s="2" t="n">
-        <v>17168</v>
-      </c>
-      <c r="D17" s="2" t="n">
-        <v>44927</v>
+      <c r="C17" t="n">
+        <v>1947</v>
+      </c>
+      <c r="D17" t="n">
+        <v>2023</v>
       </c>
       <c r="E17" t="n">
         <v>77</v>
@@ -1318,11 +1314,11 @@
           <t>Portland, ME</t>
         </is>
       </c>
-      <c r="C18" s="2" t="n">
-        <v>4384</v>
-      </c>
-      <c r="D18" s="2" t="n">
-        <v>44927</v>
+      <c r="C18" t="n">
+        <v>1912</v>
+      </c>
+      <c r="D18" t="n">
+        <v>2023</v>
       </c>
       <c r="E18" t="n">
         <v>112</v>
@@ -1368,11 +1364,11 @@
           <t>Seavey Island, ME</t>
         </is>
       </c>
-      <c r="C19" s="2" t="n">
-        <v>9498</v>
-      </c>
-      <c r="D19" s="2" t="n">
-        <v>44927</v>
+      <c r="C19" t="n">
+        <v>1926</v>
+      </c>
+      <c r="D19" t="n">
+        <v>2023</v>
       </c>
       <c r="E19" t="n">
         <v>98</v>
@@ -1418,11 +1414,11 @@
           <t>Fort Point, NH</t>
         </is>
       </c>
-      <c r="C20" s="2" t="n">
-        <v>9498</v>
-      </c>
-      <c r="D20" s="2" t="n">
-        <v>43466</v>
+      <c r="C20" t="n">
+        <v>1926</v>
+      </c>
+      <c r="D20" t="n">
+        <v>2019</v>
       </c>
       <c r="E20" t="n">
         <v>94</v>
@@ -1468,11 +1464,11 @@
           <t>Boston, MA</t>
         </is>
       </c>
-      <c r="C21" s="2" t="n">
-        <v>7672</v>
-      </c>
-      <c r="D21" s="2" t="n">
-        <v>44927</v>
+      <c r="C21" t="n">
+        <v>1921</v>
+      </c>
+      <c r="D21" t="n">
+        <v>2023</v>
       </c>
       <c r="E21" t="n">
         <v>103</v>
@@ -1518,11 +1514,11 @@
           <t>Woods Hole, MA</t>
         </is>
       </c>
-      <c r="C22" s="2" t="n">
-        <v>11689</v>
-      </c>
-      <c r="D22" s="2" t="n">
-        <v>44927</v>
+      <c r="C22" t="n">
+        <v>1932</v>
+      </c>
+      <c r="D22" t="n">
+        <v>2023</v>
       </c>
       <c r="E22" t="n">
         <v>92</v>
@@ -1568,11 +1564,11 @@
           <t>Nantucket Island, MA</t>
         </is>
       </c>
-      <c r="C23" s="2" t="n">
-        <v>23743</v>
-      </c>
-      <c r="D23" s="2" t="n">
-        <v>44927</v>
+      <c r="C23" t="n">
+        <v>1965</v>
+      </c>
+      <c r="D23" t="n">
+        <v>2023</v>
       </c>
       <c r="E23" t="n">
         <v>59</v>
@@ -1618,11 +1614,11 @@
           <t>Newport, RI</t>
         </is>
       </c>
-      <c r="C24" s="2" t="n">
-        <v>10959</v>
-      </c>
-      <c r="D24" s="2" t="n">
-        <v>44927</v>
+      <c r="C24" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D24" t="n">
+        <v>2023</v>
       </c>
       <c r="E24" t="n">
         <v>94</v>
@@ -1668,11 +1664,11 @@
           <t>Providence, RI</t>
         </is>
       </c>
-      <c r="C25" s="2" t="n">
-        <v>13881</v>
-      </c>
-      <c r="D25" s="2" t="n">
-        <v>44927</v>
+      <c r="C25" t="n">
+        <v>1938</v>
+      </c>
+      <c r="D25" t="n">
+        <v>2023</v>
       </c>
       <c r="E25" t="n">
         <v>86</v>
@@ -1718,11 +1714,11 @@
           <t>New London, CT</t>
         </is>
       </c>
-      <c r="C26" s="2" t="n">
-        <v>13881</v>
-      </c>
-      <c r="D26" s="2" t="n">
-        <v>44927</v>
+      <c r="C26" t="n">
+        <v>1938</v>
+      </c>
+      <c r="D26" t="n">
+        <v>2023</v>
       </c>
       <c r="E26" t="n">
         <v>86</v>
@@ -1768,11 +1764,11 @@
           <t>Bridgeport, CT</t>
         </is>
       </c>
-      <c r="C27" s="2" t="n">
-        <v>23377</v>
-      </c>
-      <c r="D27" s="2" t="n">
-        <v>44927</v>
+      <c r="C27" t="n">
+        <v>1964</v>
+      </c>
+      <c r="D27" t="n">
+        <v>2023</v>
       </c>
       <c r="E27" t="n">
         <v>60</v>
@@ -1818,11 +1814,11 @@
           <t>Montauk, NY</t>
         </is>
       </c>
-      <c r="C28" s="2" t="n">
-        <v>17168</v>
-      </c>
-      <c r="D28" s="2" t="n">
-        <v>44927</v>
+      <c r="C28" t="n">
+        <v>1947</v>
+      </c>
+      <c r="D28" t="n">
+        <v>2023</v>
       </c>
       <c r="E28" t="n">
         <v>77</v>
@@ -1868,11 +1864,11 @@
           <t>Kings Point, NY</t>
         </is>
       </c>
-      <c r="C29" s="2" t="n">
-        <v>11324</v>
-      </c>
-      <c r="D29" s="2" t="n">
-        <v>44927</v>
+      <c r="C29" t="n">
+        <v>1931</v>
+      </c>
+      <c r="D29" t="n">
+        <v>2023</v>
       </c>
       <c r="E29" t="n">
         <v>93</v>
@@ -1918,11 +1914,11 @@
           <t>The Battery, NY</t>
         </is>
       </c>
-      <c r="C30" s="2" t="n">
-        <v>-16069</v>
-      </c>
-      <c r="D30" s="2" t="n">
-        <v>44927</v>
+      <c r="C30" t="n">
+        <v>1856</v>
+      </c>
+      <c r="D30" t="n">
+        <v>2023</v>
       </c>
       <c r="E30" t="n">
         <v>168</v>
@@ -1968,11 +1964,11 @@
           <t>Bergen Point, NY</t>
         </is>
       </c>
-      <c r="C31" s="2" t="n">
-        <v>29587</v>
-      </c>
-      <c r="D31" s="2" t="n">
-        <v>44927</v>
+      <c r="C31" t="n">
+        <v>1981</v>
+      </c>
+      <c r="D31" t="n">
+        <v>2023</v>
       </c>
       <c r="E31" t="n">
         <v>43</v>
@@ -2018,11 +2014,11 @@
           <t>Sandy Hook, NJ</t>
         </is>
       </c>
-      <c r="C32" s="2" t="n">
-        <v>11689</v>
-      </c>
-      <c r="D32" s="2" t="n">
-        <v>44927</v>
+      <c r="C32" t="n">
+        <v>1932</v>
+      </c>
+      <c r="D32" t="n">
+        <v>2023</v>
       </c>
       <c r="E32" t="n">
         <v>92</v>
@@ -2068,11 +2064,11 @@
           <t>Atlantic City, NJ</t>
         </is>
       </c>
-      <c r="C33" s="2" t="n">
-        <v>4019</v>
-      </c>
-      <c r="D33" s="2" t="n">
-        <v>44927</v>
+      <c r="C33" t="n">
+        <v>1911</v>
+      </c>
+      <c r="D33" t="n">
+        <v>2023</v>
       </c>
       <c r="E33" t="n">
         <v>113</v>
@@ -2118,11 +2114,11 @@
           <t>Cape May, NJ</t>
         </is>
       </c>
-      <c r="C34" s="2" t="n">
-        <v>23743</v>
-      </c>
-      <c r="D34" s="2" t="n">
-        <v>44927</v>
+      <c r="C34" t="n">
+        <v>1965</v>
+      </c>
+      <c r="D34" t="n">
+        <v>2023</v>
       </c>
       <c r="E34" t="n">
         <v>59</v>
@@ -2168,11 +2164,11 @@
           <t>Philadelphia, PA</t>
         </is>
       </c>
-      <c r="C35" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D35" s="2" t="n">
-        <v>44927</v>
+      <c r="C35" t="n">
+        <v>1900</v>
+      </c>
+      <c r="D35" t="n">
+        <v>2023</v>
       </c>
       <c r="E35" t="n">
         <v>124</v>
@@ -2218,11 +2214,11 @@
           <t>Reedy Point, DE</t>
         </is>
       </c>
-      <c r="C36" s="2" t="n">
-        <v>20455</v>
-      </c>
-      <c r="D36" s="2" t="n">
-        <v>44927</v>
+      <c r="C36" t="n">
+        <v>1956</v>
+      </c>
+      <c r="D36" t="n">
+        <v>2023</v>
       </c>
       <c r="E36" t="n">
         <v>68</v>
@@ -2268,11 +2264,11 @@
           <t>Lewes, DE</t>
         </is>
       </c>
-      <c r="C37" s="2" t="n">
-        <v>6941</v>
-      </c>
-      <c r="D37" s="2" t="n">
-        <v>44927</v>
+      <c r="C37" t="n">
+        <v>1919</v>
+      </c>
+      <c r="D37" t="n">
+        <v>2023</v>
       </c>
       <c r="E37" t="n">
         <v>105</v>
@@ -2318,11 +2314,11 @@
           <t>Ocean City, MD</t>
         </is>
       </c>
-      <c r="C38" s="2" t="n">
-        <v>27395</v>
-      </c>
-      <c r="D38" s="2" t="n">
-        <v>44927</v>
+      <c r="C38" t="n">
+        <v>1975</v>
+      </c>
+      <c r="D38" t="n">
+        <v>2023</v>
       </c>
       <c r="E38" t="n">
         <v>49</v>
@@ -2368,11 +2364,11 @@
           <t>Cambridge, MD</t>
         </is>
       </c>
-      <c r="C39" s="2" t="n">
-        <v>15707</v>
-      </c>
-      <c r="D39" s="2" t="n">
-        <v>44927</v>
+      <c r="C39" t="n">
+        <v>1943</v>
+      </c>
+      <c r="D39" t="n">
+        <v>2023</v>
       </c>
       <c r="E39" t="n">
         <v>81</v>
@@ -2418,11 +2414,11 @@
           <t>Tolchester Beach, MD</t>
         </is>
       </c>
-      <c r="C40" s="2" t="n">
-        <v>25934</v>
-      </c>
-      <c r="D40" s="2" t="n">
-        <v>44927</v>
+      <c r="C40" t="n">
+        <v>1971</v>
+      </c>
+      <c r="D40" t="n">
+        <v>2023</v>
       </c>
       <c r="E40" t="n">
         <v>53</v>
@@ -2468,11 +2464,11 @@
           <t>Chesapeake City, MD</t>
         </is>
       </c>
-      <c r="C41" s="2" t="n">
-        <v>26299</v>
-      </c>
-      <c r="D41" s="2" t="n">
-        <v>44927</v>
+      <c r="C41" t="n">
+        <v>1972</v>
+      </c>
+      <c r="D41" t="n">
+        <v>2023</v>
       </c>
       <c r="E41" t="n">
         <v>52</v>
@@ -2518,11 +2514,11 @@
           <t>Baltimore, MD</t>
         </is>
       </c>
-      <c r="C42" s="2" t="n">
-        <v>732</v>
-      </c>
-      <c r="D42" s="2" t="n">
-        <v>44927</v>
+      <c r="C42" t="n">
+        <v>1902</v>
+      </c>
+      <c r="D42" t="n">
+        <v>2023</v>
       </c>
       <c r="E42" t="n">
         <v>122</v>
@@ -2568,11 +2564,11 @@
           <t>Annapolis, MD</t>
         </is>
       </c>
-      <c r="C43" s="2" t="n">
-        <v>10228</v>
-      </c>
-      <c r="D43" s="2" t="n">
-        <v>44927</v>
+      <c r="C43" t="n">
+        <v>1928</v>
+      </c>
+      <c r="D43" t="n">
+        <v>2023</v>
       </c>
       <c r="E43" t="n">
         <v>96</v>
@@ -2618,11 +2614,11 @@
           <t>Solomons Island, MD</t>
         </is>
       </c>
-      <c r="C44" s="2" t="n">
-        <v>13516</v>
-      </c>
-      <c r="D44" s="2" t="n">
-        <v>44927</v>
+      <c r="C44" t="n">
+        <v>1937</v>
+      </c>
+      <c r="D44" t="n">
+        <v>2023</v>
       </c>
       <c r="E44" t="n">
         <v>87</v>
@@ -2668,11 +2664,11 @@
           <t>Washington, DC</t>
         </is>
       </c>
-      <c r="C45" s="2" t="n">
-        <v>8767</v>
-      </c>
-      <c r="D45" s="2" t="n">
-        <v>44927</v>
+      <c r="C45" t="n">
+        <v>1924</v>
+      </c>
+      <c r="D45" t="n">
+        <v>2023</v>
       </c>
       <c r="E45" t="n">
         <v>100</v>
@@ -2718,11 +2714,11 @@
           <t>Wachapreague, VA</t>
         </is>
       </c>
-      <c r="C46" s="2" t="n">
-        <v>28491</v>
-      </c>
-      <c r="D46" s="2" t="n">
-        <v>44927</v>
+      <c r="C46" t="n">
+        <v>1978</v>
+      </c>
+      <c r="D46" t="n">
+        <v>2023</v>
       </c>
       <c r="E46" t="n">
         <v>46</v>
@@ -2768,11 +2764,11 @@
           <t>Kiptopeke, VA</t>
         </is>
       </c>
-      <c r="C47" s="2" t="n">
-        <v>18629</v>
-      </c>
-      <c r="D47" s="2" t="n">
-        <v>44927</v>
+      <c r="C47" t="n">
+        <v>1951</v>
+      </c>
+      <c r="D47" t="n">
+        <v>2023</v>
       </c>
       <c r="E47" t="n">
         <v>73</v>
@@ -2818,11 +2814,11 @@
           <t>Dahlgren, VA</t>
         </is>
       </c>
-      <c r="C48" s="2" t="n">
-        <v>26299</v>
-      </c>
-      <c r="D48" s="2" t="n">
-        <v>44927</v>
+      <c r="C48" t="n">
+        <v>1972</v>
+      </c>
+      <c r="D48" t="n">
+        <v>2023</v>
       </c>
       <c r="E48" t="n">
         <v>52</v>
@@ -2868,11 +2864,11 @@
           <t>Lewisetta, VA</t>
         </is>
       </c>
-      <c r="C49" s="2" t="n">
-        <v>25569</v>
-      </c>
-      <c r="D49" s="2" t="n">
-        <v>44927</v>
+      <c r="C49" t="n">
+        <v>1970</v>
+      </c>
+      <c r="D49" t="n">
+        <v>2023</v>
       </c>
       <c r="E49" t="n">
         <v>54</v>
@@ -2918,11 +2914,11 @@
           <t>Windmill Point, VA</t>
         </is>
       </c>
-      <c r="C50" s="2" t="n">
-        <v>29952</v>
-      </c>
-      <c r="D50" s="2" t="n">
-        <v>44927</v>
+      <c r="C50" t="n">
+        <v>1982</v>
+      </c>
+      <c r="D50" t="n">
+        <v>2023</v>
       </c>
       <c r="E50" t="n">
         <v>42</v>
@@ -2968,11 +2964,11 @@
           <t>Yorktown, VA</t>
         </is>
       </c>
-      <c r="C51" s="2" t="n">
-        <v>18264</v>
-      </c>
-      <c r="D51" s="2" t="n">
-        <v>44927</v>
+      <c r="C51" t="n">
+        <v>1950</v>
+      </c>
+      <c r="D51" t="n">
+        <v>2023</v>
       </c>
       <c r="E51" t="n">
         <v>74</v>
@@ -3018,11 +3014,11 @@
           <t>Sewells Point, VA</t>
         </is>
       </c>
-      <c r="C52" s="2" t="n">
-        <v>9863</v>
-      </c>
-      <c r="D52" s="2" t="n">
-        <v>44927</v>
+      <c r="C52" t="n">
+        <v>1927</v>
+      </c>
+      <c r="D52" t="n">
+        <v>2023</v>
       </c>
       <c r="E52" t="n">
         <v>97</v>
@@ -3068,11 +3064,11 @@
           <t>Chesapeake Bay Bridge Tunnel, VA</t>
         </is>
       </c>
-      <c r="C53" s="2" t="n">
-        <v>27395</v>
-      </c>
-      <c r="D53" s="2" t="n">
-        <v>42736</v>
+      <c r="C53" t="n">
+        <v>1975</v>
+      </c>
+      <c r="D53" t="n">
+        <v>2017</v>
       </c>
       <c r="E53" t="n">
         <v>43</v>
@@ -3118,11 +3114,11 @@
           <t>Chesapeake Channel, VA</t>
         </is>
       </c>
-      <c r="C54" s="2" t="n">
-        <v>27395</v>
-      </c>
-      <c r="D54" s="2" t="n">
-        <v>44927</v>
+      <c r="C54" t="n">
+        <v>1975</v>
+      </c>
+      <c r="D54" t="n">
+        <v>2023</v>
       </c>
       <c r="E54" t="n">
         <v>49</v>
@@ -3168,11 +3164,11 @@
           <t>Duck, NC</t>
         </is>
       </c>
-      <c r="C55" s="2" t="n">
-        <v>28491</v>
-      </c>
-      <c r="D55" s="2" t="n">
-        <v>44927</v>
+      <c r="C55" t="n">
+        <v>1978</v>
+      </c>
+      <c r="D55" t="n">
+        <v>2023</v>
       </c>
       <c r="E55" t="n">
         <v>46</v>
@@ -3218,11 +3214,11 @@
           <t>Oregon Inlet Marina, NC</t>
         </is>
       </c>
-      <c r="C56" s="2" t="n">
-        <v>28126</v>
-      </c>
-      <c r="D56" s="2" t="n">
-        <v>44927</v>
+      <c r="C56" t="n">
+        <v>1977</v>
+      </c>
+      <c r="D56" t="n">
+        <v>2023</v>
       </c>
       <c r="E56" t="n">
         <v>47</v>
@@ -3268,11 +3264,11 @@
           <t>Beaufort, NC</t>
         </is>
       </c>
-      <c r="C57" s="2" t="n">
-        <v>19360</v>
-      </c>
-      <c r="D57" s="2" t="n">
-        <v>44927</v>
+      <c r="C57" t="n">
+        <v>1953</v>
+      </c>
+      <c r="D57" t="n">
+        <v>2023</v>
       </c>
       <c r="E57" t="n">
         <v>71</v>
@@ -3318,11 +3314,11 @@
           <t>Wilmington, NC</t>
         </is>
       </c>
-      <c r="C58" s="2" t="n">
-        <v>12785</v>
-      </c>
-      <c r="D58" s="2" t="n">
-        <v>44927</v>
+      <c r="C58" t="n">
+        <v>1935</v>
+      </c>
+      <c r="D58" t="n">
+        <v>2023</v>
       </c>
       <c r="E58" t="n">
         <v>89</v>
@@ -3368,11 +3364,11 @@
           <t>Springmaid Pier, SC</t>
         </is>
       </c>
-      <c r="C59" s="2" t="n">
-        <v>20821</v>
-      </c>
-      <c r="D59" s="2" t="n">
-        <v>44927</v>
+      <c r="C59" t="n">
+        <v>1957</v>
+      </c>
+      <c r="D59" t="n">
+        <v>2023</v>
       </c>
       <c r="E59" t="n">
         <v>67</v>
@@ -3418,11 +3414,11 @@
           <t>Charleston, SC</t>
         </is>
       </c>
-      <c r="C60" s="2" t="n">
-        <v>367</v>
-      </c>
-      <c r="D60" s="2" t="n">
-        <v>44927</v>
+      <c r="C60" t="n">
+        <v>1901</v>
+      </c>
+      <c r="D60" t="n">
+        <v>2023</v>
       </c>
       <c r="E60" t="n">
         <v>123</v>
@@ -3468,11 +3464,11 @@
           <t>Fort Pulaski, GA</t>
         </is>
       </c>
-      <c r="C61" s="2" t="n">
-        <v>12785</v>
-      </c>
-      <c r="D61" s="2" t="n">
-        <v>44927</v>
+      <c r="C61" t="n">
+        <v>1935</v>
+      </c>
+      <c r="D61" t="n">
+        <v>2023</v>
       </c>
       <c r="E61" t="n">
         <v>89</v>
@@ -3518,11 +3514,11 @@
           <t>Fernandina Beach, FL</t>
         </is>
       </c>
-      <c r="C62" s="2" t="n">
-        <v>-1093</v>
-      </c>
-      <c r="D62" s="2" t="n">
-        <v>44927</v>
+      <c r="C62" t="n">
+        <v>1897</v>
+      </c>
+      <c r="D62" t="n">
+        <v>2023</v>
       </c>
       <c r="E62" t="n">
         <v>127</v>
@@ -3568,11 +3564,11 @@
           <t>Mayport, FL</t>
         </is>
       </c>
-      <c r="C63" s="2" t="n">
-        <v>10228</v>
-      </c>
-      <c r="D63" s="2" t="n">
-        <v>44927</v>
+      <c r="C63" t="n">
+        <v>1928</v>
+      </c>
+      <c r="D63" t="n">
+        <v>2023</v>
       </c>
       <c r="E63" t="n">
         <v>96</v>
@@ -3618,11 +3614,11 @@
           <t>Port Canaveral, FL</t>
         </is>
       </c>
-      <c r="C64" s="2" t="n">
-        <v>34335</v>
-      </c>
-      <c r="D64" s="2" t="n">
-        <v>44927</v>
+      <c r="C64" t="n">
+        <v>1994</v>
+      </c>
+      <c r="D64" t="n">
+        <v>2023</v>
       </c>
       <c r="E64" t="n">
         <v>30</v>
@@ -3668,11 +3664,11 @@
           <t>Lake Worth Pier, FL</t>
         </is>
       </c>
-      <c r="C65" s="2" t="n">
-        <v>25569</v>
-      </c>
-      <c r="D65" s="2" t="n">
-        <v>44927</v>
+      <c r="C65" t="n">
+        <v>1970</v>
+      </c>
+      <c r="D65" t="n">
+        <v>2023</v>
       </c>
       <c r="E65" t="n">
         <v>54</v>
@@ -3718,11 +3714,11 @@
           <t>Virginia Key, FL</t>
         </is>
       </c>
-      <c r="C66" s="2" t="n">
-        <v>11324</v>
-      </c>
-      <c r="D66" s="2" t="n">
-        <v>44927</v>
+      <c r="C66" t="n">
+        <v>1931</v>
+      </c>
+      <c r="D66" t="n">
+        <v>2023</v>
       </c>
       <c r="E66" t="n">
         <v>93</v>
@@ -3768,11 +3764,11 @@
           <t>Vaca Key, FL</t>
         </is>
       </c>
-      <c r="C67" s="2" t="n">
-        <v>25934</v>
-      </c>
-      <c r="D67" s="2" t="n">
-        <v>44927</v>
+      <c r="C67" t="n">
+        <v>1971</v>
+      </c>
+      <c r="D67" t="n">
+        <v>2023</v>
       </c>
       <c r="E67" t="n">
         <v>53</v>
@@ -3818,11 +3814,11 @@
           <t>Key West, FL</t>
         </is>
       </c>
-      <c r="C68" s="2" t="n">
-        <v>4750</v>
-      </c>
-      <c r="D68" s="2" t="n">
-        <v>44927</v>
+      <c r="C68" t="n">
+        <v>1913</v>
+      </c>
+      <c r="D68" t="n">
+        <v>2023</v>
       </c>
       <c r="E68" t="n">
         <v>111</v>
@@ -3868,11 +3864,11 @@
           <t>Naples, FL</t>
         </is>
       </c>
-      <c r="C69" s="2" t="n">
-        <v>23743</v>
-      </c>
-      <c r="D69" s="2" t="n">
-        <v>44927</v>
+      <c r="C69" t="n">
+        <v>1965</v>
+      </c>
+      <c r="D69" t="n">
+        <v>2023</v>
       </c>
       <c r="E69" t="n">
         <v>59</v>
@@ -3918,11 +3914,11 @@
           <t>Fort Myers, FL</t>
         </is>
       </c>
-      <c r="C70" s="2" t="n">
-        <v>23743</v>
-      </c>
-      <c r="D70" s="2" t="n">
-        <v>44927</v>
+      <c r="C70" t="n">
+        <v>1965</v>
+      </c>
+      <c r="D70" t="n">
+        <v>2023</v>
       </c>
       <c r="E70" t="n">
         <v>59</v>
@@ -3968,11 +3964,11 @@
           <t>Port Manatee, FL</t>
         </is>
       </c>
-      <c r="C71" s="2" t="n">
-        <v>27760</v>
-      </c>
-      <c r="D71" s="2" t="n">
-        <v>44927</v>
+      <c r="C71" t="n">
+        <v>1976</v>
+      </c>
+      <c r="D71" t="n">
+        <v>2023</v>
       </c>
       <c r="E71" t="n">
         <v>48</v>
@@ -4018,11 +4014,11 @@
           <t>St. Petersburg, FL</t>
         </is>
       </c>
-      <c r="C72" s="2" t="n">
-        <v>17168</v>
-      </c>
-      <c r="D72" s="2" t="n">
-        <v>44927</v>
+      <c r="C72" t="n">
+        <v>1947</v>
+      </c>
+      <c r="D72" t="n">
+        <v>2023</v>
       </c>
       <c r="E72" t="n">
         <v>77</v>
@@ -4068,11 +4064,11 @@
           <t>East Bay, FL</t>
         </is>
       </c>
-      <c r="C73" s="2" t="n">
-        <v>27760</v>
-      </c>
-      <c r="D73" s="2" t="n">
-        <v>44927</v>
+      <c r="C73" t="n">
+        <v>1976</v>
+      </c>
+      <c r="D73" t="n">
+        <v>2023</v>
       </c>
       <c r="E73" t="n">
         <v>48</v>
@@ -4118,11 +4114,11 @@
           <t>Clearwater Beach, FL</t>
         </is>
       </c>
-      <c r="C74" s="2" t="n">
-        <v>26665</v>
-      </c>
-      <c r="D74" s="2" t="n">
-        <v>44927</v>
+      <c r="C74" t="n">
+        <v>1973</v>
+      </c>
+      <c r="D74" t="n">
+        <v>2023</v>
       </c>
       <c r="E74" t="n">
         <v>51</v>
@@ -4168,11 +4164,11 @@
           <t>Cedar Key, FL</t>
         </is>
       </c>
-      <c r="C75" s="2" t="n">
-        <v>5115</v>
-      </c>
-      <c r="D75" s="2" t="n">
-        <v>44927</v>
+      <c r="C75" t="n">
+        <v>1914</v>
+      </c>
+      <c r="D75" t="n">
+        <v>2023</v>
       </c>
       <c r="E75" t="n">
         <v>110</v>
@@ -4218,11 +4214,11 @@
           <t>Apalachicola, FL</t>
         </is>
       </c>
-      <c r="C76" s="2" t="n">
-        <v>24473</v>
-      </c>
-      <c r="D76" s="2" t="n">
-        <v>44927</v>
+      <c r="C76" t="n">
+        <v>1967</v>
+      </c>
+      <c r="D76" t="n">
+        <v>2023</v>
       </c>
       <c r="E76" t="n">
         <v>57</v>
@@ -4268,11 +4264,11 @@
           <t>Panama City, FL</t>
         </is>
       </c>
-      <c r="C77" s="2" t="n">
-        <v>26665</v>
-      </c>
-      <c r="D77" s="2" t="n">
-        <v>44927</v>
+      <c r="C77" t="n">
+        <v>1973</v>
+      </c>
+      <c r="D77" t="n">
+        <v>2023</v>
       </c>
       <c r="E77" t="n">
         <v>51</v>
@@ -4318,11 +4314,11 @@
           <t>Panama City Beach, FL</t>
         </is>
       </c>
-      <c r="C78" s="2" t="n">
-        <v>32509</v>
-      </c>
-      <c r="D78" s="2" t="n">
-        <v>44927</v>
+      <c r="C78" t="n">
+        <v>1989</v>
+      </c>
+      <c r="D78" t="n">
+        <v>2023</v>
       </c>
       <c r="E78" t="n">
         <v>35</v>
@@ -4368,11 +4364,11 @@
           <t>Pensacola, FL</t>
         </is>
       </c>
-      <c r="C79" s="2" t="n">
-        <v>8402</v>
-      </c>
-      <c r="D79" s="2" t="n">
-        <v>44927</v>
+      <c r="C79" t="n">
+        <v>1923</v>
+      </c>
+      <c r="D79" t="n">
+        <v>2023</v>
       </c>
       <c r="E79" t="n">
         <v>101</v>
@@ -4418,11 +4414,11 @@
           <t>Dauphin Island, AL</t>
         </is>
       </c>
-      <c r="C80" s="2" t="n">
-        <v>24108</v>
-      </c>
-      <c r="D80" s="2" t="n">
-        <v>44927</v>
+      <c r="C80" t="n">
+        <v>1966</v>
+      </c>
+      <c r="D80" t="n">
+        <v>2023</v>
       </c>
       <c r="E80" t="n">
         <v>58</v>
@@ -4468,11 +4464,11 @@
           <t>Mobile State Docks, AL</t>
         </is>
       </c>
-      <c r="C81" s="2" t="n">
-        <v>29221</v>
-      </c>
-      <c r="D81" s="2" t="n">
-        <v>44927</v>
+      <c r="C81" t="n">
+        <v>1980</v>
+      </c>
+      <c r="D81" t="n">
+        <v>2023</v>
       </c>
       <c r="E81" t="n">
         <v>44</v>
@@ -4518,11 +4514,11 @@
           <t>Bay Waveland, MS</t>
         </is>
       </c>
-      <c r="C82" s="2" t="n">
-        <v>28491</v>
-      </c>
-      <c r="D82" s="2" t="n">
-        <v>44927</v>
+      <c r="C82" t="n">
+        <v>1978</v>
+      </c>
+      <c r="D82" t="n">
+        <v>2023</v>
       </c>
       <c r="E82" t="n">
         <v>46</v>
@@ -4568,11 +4564,11 @@
           <t>Grand Isle, LA</t>
         </is>
       </c>
-      <c r="C83" s="2" t="n">
-        <v>17168</v>
-      </c>
-      <c r="D83" s="2" t="n">
-        <v>44927</v>
+      <c r="C83" t="n">
+        <v>1947</v>
+      </c>
+      <c r="D83" t="n">
+        <v>2023</v>
       </c>
       <c r="E83" t="n">
         <v>77</v>
@@ -4618,11 +4614,11 @@
           <t>New Canal, LA</t>
         </is>
       </c>
-      <c r="C84" s="2" t="n">
-        <v>29952</v>
-      </c>
-      <c r="D84" s="2" t="n">
-        <v>44927</v>
+      <c r="C84" t="n">
+        <v>1982</v>
+      </c>
+      <c r="D84" t="n">
+        <v>2023</v>
       </c>
       <c r="E84" t="n">
         <v>42</v>
@@ -4668,11 +4664,11 @@
           <t>Sabine Pass, TX</t>
         </is>
       </c>
-      <c r="C85" s="2" t="n">
-        <v>21186</v>
-      </c>
-      <c r="D85" s="2" t="n">
-        <v>43831</v>
+      <c r="C85" t="n">
+        <v>1958</v>
+      </c>
+      <c r="D85" t="n">
+        <v>2020</v>
       </c>
       <c r="E85" t="n">
         <v>63</v>
@@ -4718,11 +4714,11 @@
           <t>Morgans Point, TX</t>
         </is>
       </c>
-      <c r="C86" s="2" t="n">
-        <v>33970</v>
-      </c>
-      <c r="D86" s="2" t="n">
-        <v>44927</v>
+      <c r="C86" t="n">
+        <v>1993</v>
+      </c>
+      <c r="D86" t="n">
+        <v>2023</v>
       </c>
       <c r="E86" t="n">
         <v>31</v>
@@ -4768,11 +4764,11 @@
           <t>Texas Point, TX</t>
         </is>
       </c>
-      <c r="C87" s="2" t="n">
-        <v>21186</v>
-      </c>
-      <c r="D87" s="2" t="n">
-        <v>44927</v>
+      <c r="C87" t="n">
+        <v>1958</v>
+      </c>
+      <c r="D87" t="n">
+        <v>2023</v>
       </c>
       <c r="E87" t="n">
         <v>66</v>
@@ -4818,11 +4814,11 @@
           <t>Eagle Point, TX</t>
         </is>
       </c>
-      <c r="C88" s="2" t="n">
-        <v>33970</v>
-      </c>
-      <c r="D88" s="2" t="n">
-        <v>44927</v>
+      <c r="C88" t="n">
+        <v>1993</v>
+      </c>
+      <c r="D88" t="n">
+        <v>2023</v>
       </c>
       <c r="E88" t="n">
         <v>31</v>
@@ -4868,11 +4864,11 @@
           <t>Galveston Bay Entrance, TX</t>
         </is>
       </c>
-      <c r="C89" s="2" t="n">
-        <v>20821</v>
-      </c>
-      <c r="D89" s="2" t="n">
-        <v>44927</v>
+      <c r="C89" t="n">
+        <v>1957</v>
+      </c>
+      <c r="D89" t="n">
+        <v>2023</v>
       </c>
       <c r="E89" t="n">
         <v>67</v>
@@ -4918,11 +4914,11 @@
           <t>Galveston Pier 21, TX</t>
         </is>
       </c>
-      <c r="C90" s="2" t="n">
-        <v>1462</v>
-      </c>
-      <c r="D90" s="2" t="n">
-        <v>44927</v>
+      <c r="C90" t="n">
+        <v>1904</v>
+      </c>
+      <c r="D90" t="n">
+        <v>2023</v>
       </c>
       <c r="E90" t="n">
         <v>120</v>
@@ -4968,11 +4964,11 @@
           <t>Galveston Pleasure Pier, TX</t>
         </is>
       </c>
-      <c r="C91" s="2" t="n">
-        <v>20821</v>
-      </c>
-      <c r="D91" s="2" t="n">
-        <v>40544</v>
+      <c r="C91" t="n">
+        <v>1957</v>
+      </c>
+      <c r="D91" t="n">
+        <v>2011</v>
       </c>
       <c r="E91" t="n">
         <v>55</v>
@@ -5018,11 +5014,11 @@
           <t>Freeport Harbor, TX</t>
         </is>
       </c>
-      <c r="C92" s="2" t="n">
-        <v>19725</v>
-      </c>
-      <c r="D92" s="2" t="n">
-        <v>44927</v>
+      <c r="C92" t="n">
+        <v>1954</v>
+      </c>
+      <c r="D92" t="n">
+        <v>2023</v>
       </c>
       <c r="E92" t="n">
         <v>52</v>
@@ -5068,11 +5064,11 @@
           <t>Rockport, TX</t>
         </is>
       </c>
-      <c r="C93" s="2" t="n">
-        <v>13516</v>
-      </c>
-      <c r="D93" s="2" t="n">
-        <v>44927</v>
+      <c r="C93" t="n">
+        <v>1937</v>
+      </c>
+      <c r="D93" t="n">
+        <v>2023</v>
       </c>
       <c r="E93" t="n">
         <v>87</v>
@@ -5118,11 +5114,11 @@
           <t>Corpus Christi, TX</t>
         </is>
       </c>
-      <c r="C94" s="2" t="n">
-        <v>30317</v>
-      </c>
-      <c r="D94" s="2" t="n">
-        <v>44562</v>
+      <c r="C94" t="n">
+        <v>1983</v>
+      </c>
+      <c r="D94" t="n">
+        <v>2022</v>
       </c>
       <c r="E94" t="n">
         <v>40</v>
@@ -5168,11 +5164,11 @@
           <t>Port Mansfield, TX</t>
         </is>
       </c>
-      <c r="C95" s="2" t="n">
-        <v>23012</v>
-      </c>
-      <c r="D95" s="2" t="n">
-        <v>44927</v>
+      <c r="C95" t="n">
+        <v>1963</v>
+      </c>
+      <c r="D95" t="n">
+        <v>2023</v>
       </c>
       <c r="E95" t="n">
         <v>61</v>
@@ -5218,11 +5214,11 @@
           <t>South Padre Island, TX</t>
         </is>
       </c>
-      <c r="C96" s="2" t="n">
-        <v>21186</v>
-      </c>
-      <c r="D96" s="2" t="n">
-        <v>44927</v>
+      <c r="C96" t="n">
+        <v>1958</v>
+      </c>
+      <c r="D96" t="n">
+        <v>2023</v>
       </c>
       <c r="E96" t="n">
         <v>66</v>
@@ -5268,11 +5264,11 @@
           <t>Port Isabel, TX</t>
         </is>
       </c>
-      <c r="C97" s="2" t="n">
-        <v>16072</v>
-      </c>
-      <c r="D97" s="2" t="n">
-        <v>44927</v>
+      <c r="C97" t="n">
+        <v>1944</v>
+      </c>
+      <c r="D97" t="n">
+        <v>2023</v>
       </c>
       <c r="E97" t="n">
         <v>80</v>
@@ -5318,11 +5314,11 @@
           <t>San Diego, CA</t>
         </is>
       </c>
-      <c r="C98" s="2" t="n">
-        <v>2193</v>
-      </c>
-      <c r="D98" s="2" t="n">
-        <v>44927</v>
+      <c r="C98" t="n">
+        <v>1906</v>
+      </c>
+      <c r="D98" t="n">
+        <v>2023</v>
       </c>
       <c r="E98" t="n">
         <v>118</v>
@@ -5368,11 +5364,11 @@
           <t>La Jolla, CA</t>
         </is>
       </c>
-      <c r="C99" s="2" t="n">
-        <v>8767</v>
-      </c>
-      <c r="D99" s="2" t="n">
-        <v>44927</v>
+      <c r="C99" t="n">
+        <v>1924</v>
+      </c>
+      <c r="D99" t="n">
+        <v>2023</v>
       </c>
       <c r="E99" t="n">
         <v>100</v>
@@ -5418,11 +5414,11 @@
           <t>Los Angeles, CA</t>
         </is>
       </c>
-      <c r="C100" s="2" t="n">
-        <v>8402</v>
-      </c>
-      <c r="D100" s="2" t="n">
-        <v>44927</v>
+      <c r="C100" t="n">
+        <v>1923</v>
+      </c>
+      <c r="D100" t="n">
+        <v>2023</v>
       </c>
       <c r="E100" t="n">
         <v>101</v>
@@ -5468,11 +5464,11 @@
           <t>Santa Monica, CA</t>
         </is>
       </c>
-      <c r="C101" s="2" t="n">
-        <v>12055</v>
-      </c>
-      <c r="D101" s="2" t="n">
-        <v>44927</v>
+      <c r="C101" t="n">
+        <v>1933</v>
+      </c>
+      <c r="D101" t="n">
+        <v>2023</v>
       </c>
       <c r="E101" t="n">
         <v>91</v>
@@ -5518,11 +5514,11 @@
           <t>Santa Barbara, CA</t>
         </is>
       </c>
-      <c r="C102" s="2" t="n">
-        <v>26665</v>
-      </c>
-      <c r="D102" s="2" t="n">
-        <v>44927</v>
+      <c r="C102" t="n">
+        <v>1973</v>
+      </c>
+      <c r="D102" t="n">
+        <v>2023</v>
       </c>
       <c r="E102" t="n">
         <v>51</v>
@@ -5568,11 +5564,11 @@
           <t>Port San Luis, CA</t>
         </is>
       </c>
-      <c r="C103" s="2" t="n">
-        <v>16438</v>
-      </c>
-      <c r="D103" s="2" t="n">
-        <v>44927</v>
+      <c r="C103" t="n">
+        <v>1945</v>
+      </c>
+      <c r="D103" t="n">
+        <v>2023</v>
       </c>
       <c r="E103" t="n">
         <v>79</v>
@@ -5618,11 +5614,11 @@
           <t>Monterey, CA</t>
         </is>
       </c>
-      <c r="C104" s="2" t="n">
-        <v>26665</v>
-      </c>
-      <c r="D104" s="2" t="n">
-        <v>44927</v>
+      <c r="C104" t="n">
+        <v>1973</v>
+      </c>
+      <c r="D104" t="n">
+        <v>2023</v>
       </c>
       <c r="E104" t="n">
         <v>51</v>
@@ -5668,11 +5664,11 @@
           <t>San Francisco, CA</t>
         </is>
       </c>
-      <c r="C105" s="2" t="n">
-        <v>-1093</v>
-      </c>
-      <c r="D105" s="2" t="n">
-        <v>44927</v>
+      <c r="C105" t="n">
+        <v>1897</v>
+      </c>
+      <c r="D105" t="n">
+        <v>2023</v>
       </c>
       <c r="E105" t="n">
         <v>127</v>
@@ -5718,11 +5714,11 @@
           <t>Redwood City, CA</t>
         </is>
       </c>
-      <c r="C106" s="2" t="n">
-        <v>27030</v>
-      </c>
-      <c r="D106" s="2" t="n">
-        <v>44927</v>
+      <c r="C106" t="n">
+        <v>1974</v>
+      </c>
+      <c r="D106" t="n">
+        <v>2023</v>
       </c>
       <c r="E106" t="n">
         <v>50</v>
@@ -5768,11 +5764,11 @@
           <t>Alameda, CA</t>
         </is>
       </c>
-      <c r="C107" s="2" t="n">
-        <v>14246</v>
-      </c>
-      <c r="D107" s="2" t="n">
-        <v>44927</v>
+      <c r="C107" t="n">
+        <v>1939</v>
+      </c>
+      <c r="D107" t="n">
+        <v>2023</v>
       </c>
       <c r="E107" t="n">
         <v>85</v>
@@ -5818,11 +5814,11 @@
           <t>Point Reyes, CA</t>
         </is>
       </c>
-      <c r="C108" s="2" t="n">
-        <v>27395</v>
-      </c>
-      <c r="D108" s="2" t="n">
-        <v>44927</v>
+      <c r="C108" t="n">
+        <v>1975</v>
+      </c>
+      <c r="D108" t="n">
+        <v>2023</v>
       </c>
       <c r="E108" t="n">
         <v>49</v>
@@ -5868,11 +5864,11 @@
           <t>Port Chicago, CA</t>
         </is>
       </c>
-      <c r="C109" s="2" t="n">
-        <v>27760</v>
-      </c>
-      <c r="D109" s="2" t="n">
-        <v>44927</v>
+      <c r="C109" t="n">
+        <v>1976</v>
+      </c>
+      <c r="D109" t="n">
+        <v>2023</v>
       </c>
       <c r="E109" t="n">
         <v>48</v>
@@ -5918,11 +5914,11 @@
           <t>Arena Cove, CA</t>
         </is>
       </c>
-      <c r="C110" s="2" t="n">
-        <v>28491</v>
-      </c>
-      <c r="D110" s="2" t="n">
-        <v>44927</v>
+      <c r="C110" t="n">
+        <v>1978</v>
+      </c>
+      <c r="D110" t="n">
+        <v>2023</v>
       </c>
       <c r="E110" t="n">
         <v>46</v>
@@ -5968,11 +5964,11 @@
           <t>North Spit, CA</t>
         </is>
       </c>
-      <c r="C111" s="2" t="n">
-        <v>28126</v>
-      </c>
-      <c r="D111" s="2" t="n">
-        <v>44927</v>
+      <c r="C111" t="n">
+        <v>1977</v>
+      </c>
+      <c r="D111" t="n">
+        <v>2023</v>
       </c>
       <c r="E111" t="n">
         <v>47</v>
@@ -6018,11 +6014,11 @@
           <t>Crescent City, CA</t>
         </is>
       </c>
-      <c r="C112" s="2" t="n">
-        <v>12055</v>
-      </c>
-      <c r="D112" s="2" t="n">
-        <v>44927</v>
+      <c r="C112" t="n">
+        <v>1933</v>
+      </c>
+      <c r="D112" t="n">
+        <v>2023</v>
       </c>
       <c r="E112" t="n">
         <v>91</v>
@@ -6068,11 +6064,11 @@
           <t>Port Orford, OR</t>
         </is>
       </c>
-      <c r="C113" s="2" t="n">
-        <v>28126</v>
-      </c>
-      <c r="D113" s="2" t="n">
-        <v>44927</v>
+      <c r="C113" t="n">
+        <v>1977</v>
+      </c>
+      <c r="D113" t="n">
+        <v>2023</v>
       </c>
       <c r="E113" t="n">
         <v>47</v>
@@ -6118,11 +6114,11 @@
           <t>Charleston, OR</t>
         </is>
       </c>
-      <c r="C114" s="2" t="n">
-        <v>25569</v>
-      </c>
-      <c r="D114" s="2" t="n">
-        <v>44927</v>
+      <c r="C114" t="n">
+        <v>1970</v>
+      </c>
+      <c r="D114" t="n">
+        <v>2023</v>
       </c>
       <c r="E114" t="n">
         <v>54</v>
@@ -6168,11 +6164,11 @@
           <t>South Beach, OR</t>
         </is>
       </c>
-      <c r="C115" s="2" t="n">
-        <v>24473</v>
-      </c>
-      <c r="D115" s="2" t="n">
-        <v>44927</v>
+      <c r="C115" t="n">
+        <v>1967</v>
+      </c>
+      <c r="D115" t="n">
+        <v>2023</v>
       </c>
       <c r="E115" t="n">
         <v>57</v>
@@ -6218,11 +6214,11 @@
           <t>Garibaldi, OR</t>
         </is>
       </c>
-      <c r="C116" s="2" t="n">
-        <v>25569</v>
-      </c>
-      <c r="D116" s="2" t="n">
-        <v>44927</v>
+      <c r="C116" t="n">
+        <v>1970</v>
+      </c>
+      <c r="D116" t="n">
+        <v>2023</v>
       </c>
       <c r="E116" t="n">
         <v>54</v>
@@ -6268,11 +6264,11 @@
           <t>Astoria, OR</t>
         </is>
       </c>
-      <c r="C117" s="2" t="n">
-        <v>9133</v>
-      </c>
-      <c r="D117" s="2" t="n">
-        <v>44927</v>
+      <c r="C117" t="n">
+        <v>1925</v>
+      </c>
+      <c r="D117" t="n">
+        <v>2023</v>
       </c>
       <c r="E117" t="n">
         <v>99</v>
@@ -6318,11 +6314,11 @@
           <t>Toke Point, WA</t>
         </is>
       </c>
-      <c r="C118" s="2" t="n">
-        <v>26665</v>
-      </c>
-      <c r="D118" s="2" t="n">
-        <v>44927</v>
+      <c r="C118" t="n">
+        <v>1973</v>
+      </c>
+      <c r="D118" t="n">
+        <v>2023</v>
       </c>
       <c r="E118" t="n">
         <v>51</v>
@@ -6368,11 +6364,11 @@
           <t>Neah Bay, WA</t>
         </is>
       </c>
-      <c r="C119" s="2" t="n">
-        <v>12420</v>
-      </c>
-      <c r="D119" s="2" t="n">
-        <v>44927</v>
+      <c r="C119" t="n">
+        <v>1934</v>
+      </c>
+      <c r="D119" t="n">
+        <v>2023</v>
       </c>
       <c r="E119" t="n">
         <v>90</v>
@@ -6418,11 +6414,11 @@
           <t>Port Angeles, WA</t>
         </is>
       </c>
-      <c r="C120" s="2" t="n">
-        <v>27395</v>
-      </c>
-      <c r="D120" s="2" t="n">
-        <v>44927</v>
+      <c r="C120" t="n">
+        <v>1975</v>
+      </c>
+      <c r="D120" t="n">
+        <v>2023</v>
       </c>
       <c r="E120" t="n">
         <v>49</v>
@@ -6468,11 +6464,11 @@
           <t>Port Townsend, WA</t>
         </is>
       </c>
-      <c r="C121" s="2" t="n">
-        <v>26299</v>
-      </c>
-      <c r="D121" s="2" t="n">
-        <v>44927</v>
+      <c r="C121" t="n">
+        <v>1972</v>
+      </c>
+      <c r="D121" t="n">
+        <v>2023</v>
       </c>
       <c r="E121" t="n">
         <v>52</v>
@@ -6518,11 +6514,11 @@
           <t>Seattle, WA</t>
         </is>
       </c>
-      <c r="C122" s="2" t="n">
-        <v>-363</v>
-      </c>
-      <c r="D122" s="2" t="n">
-        <v>44927</v>
+      <c r="C122" t="n">
+        <v>1899</v>
+      </c>
+      <c r="D122" t="n">
+        <v>2023</v>
       </c>
       <c r="E122" t="n">
         <v>125</v>
@@ -6568,11 +6564,11 @@
           <t>Cherry Point, WA</t>
         </is>
       </c>
-      <c r="C123" s="2" t="n">
-        <v>26665</v>
-      </c>
-      <c r="D123" s="2" t="n">
-        <v>44927</v>
+      <c r="C123" t="n">
+        <v>1973</v>
+      </c>
+      <c r="D123" t="n">
+        <v>2023</v>
       </c>
       <c r="E123" t="n">
         <v>51</v>
@@ -6618,11 +6614,11 @@
           <t>Friday Harbor, WA</t>
         </is>
       </c>
-      <c r="C124" s="2" t="n">
-        <v>12420</v>
-      </c>
-      <c r="D124" s="2" t="n">
-        <v>44927</v>
+      <c r="C124" t="n">
+        <v>1934</v>
+      </c>
+      <c r="D124" t="n">
+        <v>2023</v>
       </c>
       <c r="E124" t="n">
         <v>90</v>
@@ -6668,11 +6664,11 @@
           <t>Ketchikan, AK</t>
         </is>
       </c>
-      <c r="C125" s="2" t="n">
-        <v>6941</v>
-      </c>
-      <c r="D125" s="2" t="n">
-        <v>44927</v>
+      <c r="C125" t="n">
+        <v>1919</v>
+      </c>
+      <c r="D125" t="n">
+        <v>2023</v>
       </c>
       <c r="E125" t="n">
         <v>105</v>
@@ -6718,11 +6714,11 @@
           <t>Sitka, AK</t>
         </is>
       </c>
-      <c r="C126" s="2" t="n">
-        <v>8767</v>
-      </c>
-      <c r="D126" s="2" t="n">
-        <v>44927</v>
+      <c r="C126" t="n">
+        <v>1924</v>
+      </c>
+      <c r="D126" t="n">
+        <v>2023</v>
       </c>
       <c r="E126" t="n">
         <v>100</v>
@@ -6768,11 +6764,11 @@
           <t>Juneau, AK</t>
         </is>
       </c>
-      <c r="C127" s="2" t="n">
-        <v>13150</v>
-      </c>
-      <c r="D127" s="2" t="n">
-        <v>44927</v>
+      <c r="C127" t="n">
+        <v>1936</v>
+      </c>
+      <c r="D127" t="n">
+        <v>2023</v>
       </c>
       <c r="E127" t="n">
         <v>88</v>
@@ -6818,11 +6814,11 @@
           <t>Skagway, AK</t>
         </is>
       </c>
-      <c r="C128" s="2" t="n">
-        <v>16072</v>
-      </c>
-      <c r="D128" s="2" t="n">
-        <v>44927</v>
+      <c r="C128" t="n">
+        <v>1944</v>
+      </c>
+      <c r="D128" t="n">
+        <v>2023</v>
       </c>
       <c r="E128" t="n">
         <v>80</v>
@@ -6868,11 +6864,11 @@
           <t>Yakutat, AK</t>
         </is>
       </c>
-      <c r="C129" s="2" t="n">
-        <v>32143</v>
-      </c>
-      <c r="D129" s="2" t="n">
-        <v>44927</v>
+      <c r="C129" t="n">
+        <v>1988</v>
+      </c>
+      <c r="D129" t="n">
+        <v>2023</v>
       </c>
       <c r="E129" t="n">
         <v>36</v>
@@ -6918,11 +6914,11 @@
           <t>Cordova, AK</t>
         </is>
       </c>
-      <c r="C130" s="2" t="n">
-        <v>32143</v>
-      </c>
-      <c r="D130" s="2" t="n">
-        <v>44927</v>
+      <c r="C130" t="n">
+        <v>1988</v>
+      </c>
+      <c r="D130" t="n">
+        <v>2023</v>
       </c>
       <c r="E130" t="n">
         <v>36</v>
@@ -6968,11 +6964,11 @@
           <t>Valdez, AK</t>
         </is>
       </c>
-      <c r="C131" s="2" t="n">
-        <v>32143</v>
-      </c>
-      <c r="D131" s="2" t="n">
-        <v>44927</v>
+      <c r="C131" t="n">
+        <v>1988</v>
+      </c>
+      <c r="D131" t="n">
+        <v>2023</v>
       </c>
       <c r="E131" t="n">
         <v>36</v>
@@ -7018,11 +7014,11 @@
           <t>Seward, AK</t>
         </is>
       </c>
-      <c r="C132" s="2" t="n">
-        <v>23377</v>
-      </c>
-      <c r="D132" s="2" t="n">
-        <v>44927</v>
+      <c r="C132" t="n">
+        <v>1964</v>
+      </c>
+      <c r="D132" t="n">
+        <v>2023</v>
       </c>
       <c r="E132" t="n">
         <v>60</v>
@@ -7068,11 +7064,11 @@
           <t>Seldovia, AK</t>
         </is>
       </c>
-      <c r="C133" s="2" t="n">
-        <v>23377</v>
-      </c>
-      <c r="D133" s="2" t="n">
-        <v>44927</v>
+      <c r="C133" t="n">
+        <v>1964</v>
+      </c>
+      <c r="D133" t="n">
+        <v>2023</v>
       </c>
       <c r="E133" t="n">
         <v>60</v>
@@ -7118,11 +7114,11 @@
           <t>Nikiski, AK</t>
         </is>
       </c>
-      <c r="C134" s="2" t="n">
-        <v>26665</v>
-      </c>
-      <c r="D134" s="2" t="n">
-        <v>44927</v>
+      <c r="C134" t="n">
+        <v>1973</v>
+      </c>
+      <c r="D134" t="n">
+        <v>2023</v>
       </c>
       <c r="E134" t="n">
         <v>51</v>
@@ -7168,11 +7164,11 @@
           <t>Anchorage, AK</t>
         </is>
       </c>
-      <c r="C135" s="2" t="n">
-        <v>26299</v>
-      </c>
-      <c r="D135" s="2" t="n">
-        <v>44927</v>
+      <c r="C135" t="n">
+        <v>1972</v>
+      </c>
+      <c r="D135" t="n">
+        <v>2023</v>
       </c>
       <c r="E135" t="n">
         <v>52</v>
@@ -7218,11 +7214,11 @@
           <t>Kodiak Island, AK</t>
         </is>
       </c>
-      <c r="C136" s="2" t="n">
-        <v>23377</v>
-      </c>
-      <c r="D136" s="2" t="n">
-        <v>44927</v>
+      <c r="C136" t="n">
+        <v>1964</v>
+      </c>
+      <c r="D136" t="n">
+        <v>2023</v>
       </c>
       <c r="E136" t="n">
         <v>60</v>
@@ -7268,11 +7264,11 @@
           <t>Sand Point, AK</t>
         </is>
       </c>
-      <c r="C137" s="2" t="n">
-        <v>26299</v>
-      </c>
-      <c r="D137" s="2" t="n">
-        <v>44927</v>
+      <c r="C137" t="n">
+        <v>1972</v>
+      </c>
+      <c r="D137" t="n">
+        <v>2023</v>
       </c>
       <c r="E137" t="n">
         <v>52</v>
@@ -7318,11 +7314,11 @@
           <t>Adak Island, AK</t>
         </is>
       </c>
-      <c r="C138" s="2" t="n">
-        <v>20821</v>
-      </c>
-      <c r="D138" s="2" t="n">
-        <v>44927</v>
+      <c r="C138" t="n">
+        <v>1957</v>
+      </c>
+      <c r="D138" t="n">
+        <v>2023</v>
       </c>
       <c r="E138" t="n">
         <v>67</v>
@@ -7368,11 +7364,11 @@
           <t>Unalaska, AK</t>
         </is>
       </c>
-      <c r="C139" s="2" t="n">
-        <v>20821</v>
-      </c>
-      <c r="D139" s="2" t="n">
-        <v>44927</v>
+      <c r="C139" t="n">
+        <v>1957</v>
+      </c>
+      <c r="D139" t="n">
+        <v>2023</v>
       </c>
       <c r="E139" t="n">
         <v>67</v>
@@ -7418,11 +7414,11 @@
           <t>Port Moller, AK</t>
         </is>
       </c>
-      <c r="C140" s="2" t="n">
-        <v>30682</v>
-      </c>
-      <c r="D140" s="2" t="n">
-        <v>44927</v>
+      <c r="C140" t="n">
+        <v>1984</v>
+      </c>
+      <c r="D140" t="n">
+        <v>2023</v>
       </c>
       <c r="E140" t="n">
         <v>40</v>
@@ -7468,11 +7464,11 @@
           <t>Nome, AK</t>
         </is>
       </c>
-      <c r="C141" s="2" t="n">
-        <v>33604</v>
-      </c>
-      <c r="D141" s="2" t="n">
-        <v>44927</v>
+      <c r="C141" t="n">
+        <v>1992</v>
+      </c>
+      <c r="D141" t="n">
+        <v>2023</v>
       </c>
       <c r="E141" t="n">
         <v>32</v>
@@ -7518,11 +7514,11 @@
           <t>Prudhoe Bay, AK</t>
         </is>
       </c>
-      <c r="C142" s="2" t="n">
-        <v>32143</v>
-      </c>
-      <c r="D142" s="2" t="n">
-        <v>44927</v>
+      <c r="C142" t="n">
+        <v>1988</v>
+      </c>
+      <c r="D142" t="n">
+        <v>2023</v>
       </c>
       <c r="E142" t="n">
         <v>36</v>
@@ -7568,11 +7564,11 @@
           <t>Lime Tree Bay, VI</t>
         </is>
       </c>
-      <c r="C143" s="2" t="n">
-        <v>28126</v>
-      </c>
-      <c r="D143" s="2" t="n">
-        <v>44927</v>
+      <c r="C143" t="n">
+        <v>1977</v>
+      </c>
+      <c r="D143" t="n">
+        <v>2023</v>
       </c>
       <c r="E143" t="n">
         <v>47</v>
@@ -7618,11 +7614,11 @@
           <t>Charlotte Amalie, VI</t>
         </is>
       </c>
-      <c r="C144" s="2" t="n">
-        <v>27395</v>
-      </c>
-      <c r="D144" s="2" t="n">
-        <v>44927</v>
+      <c r="C144" t="n">
+        <v>1975</v>
+      </c>
+      <c r="D144" t="n">
+        <v>2023</v>
       </c>
       <c r="E144" t="n">
         <v>49</v>
@@ -7668,11 +7664,11 @@
           <t>San Juan, PR</t>
         </is>
       </c>
-      <c r="C145" s="2" t="n">
-        <v>22647</v>
-      </c>
-      <c r="D145" s="2" t="n">
-        <v>44927</v>
+      <c r="C145" t="n">
+        <v>1962</v>
+      </c>
+      <c r="D145" t="n">
+        <v>2023</v>
       </c>
       <c r="E145" t="n">
         <v>62</v>
@@ -7718,11 +7714,11 @@
           <t>Magueyes Island, PR</t>
         </is>
       </c>
-      <c r="C146" s="2" t="n">
-        <v>20090</v>
-      </c>
-      <c r="D146" s="2" t="n">
-        <v>44927</v>
+      <c r="C146" t="n">
+        <v>1955</v>
+      </c>
+      <c r="D146" t="n">
+        <v>2023</v>
       </c>
       <c r="E146" t="n">
         <v>69</v>

</xml_diff>

<commit_message>
Update data files and remove unused column_names.txt
</commit_message>
<xml_diff>
--- a/data/usstations.xlsx
+++ b/data/usstations.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N146"/>
+  <dimension ref="A1:O146"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -504,6 +504,11 @@
           <t>State</t>
         </is>
       </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Region</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -554,6 +559,11 @@
           <t>HI</t>
         </is>
       </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -604,6 +614,11 @@
           <t>HI</t>
         </is>
       </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -654,6 +669,11 @@
           <t>HI</t>
         </is>
       </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -704,6 +724,11 @@
           <t>HI</t>
         </is>
       </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -754,6 +779,11 @@
           <t>HI</t>
         </is>
       </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -804,6 +834,11 @@
           <t>HI</t>
         </is>
       </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -854,6 +889,11 @@
           <t>Unknown</t>
         </is>
       </c>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -904,6 +944,11 @@
           <t>Guam</t>
         </is>
       </c>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -954,6 +999,11 @@
           <t>American Samoa</t>
         </is>
       </c>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -1004,6 +1054,11 @@
           <t>Marshall Islands</t>
         </is>
       </c>
+      <c r="O11" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -1054,6 +1109,11 @@
           <t>Pacific Ocean</t>
         </is>
       </c>
+      <c r="O12" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -1104,6 +1164,11 @@
           <t>Bermuda</t>
         </is>
       </c>
+      <c r="O13" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -1154,6 +1219,11 @@
           <t>Bermuda</t>
         </is>
       </c>
+      <c r="O14" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -1204,6 +1274,11 @@
           <t>ME</t>
         </is>
       </c>
+      <c r="O15" t="inlineStr">
+        <is>
+          <t>East Coast</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -1254,6 +1329,11 @@
           <t>ME</t>
         </is>
       </c>
+      <c r="O16" t="inlineStr">
+        <is>
+          <t>East Coast</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -1304,6 +1384,11 @@
           <t>ME</t>
         </is>
       </c>
+      <c r="O17" t="inlineStr">
+        <is>
+          <t>East Coast</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
@@ -1354,6 +1439,11 @@
           <t>ME</t>
         </is>
       </c>
+      <c r="O18" t="inlineStr">
+        <is>
+          <t>East Coast</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
@@ -1404,6 +1494,11 @@
           <t>ME</t>
         </is>
       </c>
+      <c r="O19" t="inlineStr">
+        <is>
+          <t>East Coast</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
@@ -1454,6 +1549,11 @@
           <t>NH</t>
         </is>
       </c>
+      <c r="O20" t="inlineStr">
+        <is>
+          <t>East Coast</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
@@ -1504,6 +1604,11 @@
           <t>MA</t>
         </is>
       </c>
+      <c r="O21" t="inlineStr">
+        <is>
+          <t>East Coast</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
@@ -1554,6 +1659,11 @@
           <t>MA</t>
         </is>
       </c>
+      <c r="O22" t="inlineStr">
+        <is>
+          <t>East Coast</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
@@ -1604,6 +1714,11 @@
           <t>MA</t>
         </is>
       </c>
+      <c r="O23" t="inlineStr">
+        <is>
+          <t>East Coast</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
@@ -1654,6 +1769,11 @@
           <t>RI</t>
         </is>
       </c>
+      <c r="O24" t="inlineStr">
+        <is>
+          <t>East Coast</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
@@ -1704,6 +1824,11 @@
           <t>RI</t>
         </is>
       </c>
+      <c r="O25" t="inlineStr">
+        <is>
+          <t>East Coast</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
@@ -1754,6 +1879,11 @@
           <t>CT</t>
         </is>
       </c>
+      <c r="O26" t="inlineStr">
+        <is>
+          <t>East Coast</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
@@ -1804,6 +1934,11 @@
           <t>CT</t>
         </is>
       </c>
+      <c r="O27" t="inlineStr">
+        <is>
+          <t>East Coast</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
@@ -1854,6 +1989,11 @@
           <t>NY</t>
         </is>
       </c>
+      <c r="O28" t="inlineStr">
+        <is>
+          <t>East Coast</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
@@ -1904,6 +2044,11 @@
           <t>NY</t>
         </is>
       </c>
+      <c r="O29" t="inlineStr">
+        <is>
+          <t>East Coast</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
@@ -1954,6 +2099,11 @@
           <t>NY</t>
         </is>
       </c>
+      <c r="O30" t="inlineStr">
+        <is>
+          <t>East Coast</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
@@ -2004,6 +2154,11 @@
           <t>NY</t>
         </is>
       </c>
+      <c r="O31" t="inlineStr">
+        <is>
+          <t>East Coast</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
@@ -2054,6 +2209,11 @@
           <t>NJ</t>
         </is>
       </c>
+      <c r="O32" t="inlineStr">
+        <is>
+          <t>East Coast</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
@@ -2104,6 +2264,11 @@
           <t>NJ</t>
         </is>
       </c>
+      <c r="O33" t="inlineStr">
+        <is>
+          <t>East Coast</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
@@ -2154,6 +2319,11 @@
           <t>NJ</t>
         </is>
       </c>
+      <c r="O34" t="inlineStr">
+        <is>
+          <t>East Coast</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
@@ -2204,6 +2374,11 @@
           <t>PA</t>
         </is>
       </c>
+      <c r="O35" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
@@ -2254,6 +2429,11 @@
           <t>DE</t>
         </is>
       </c>
+      <c r="O36" t="inlineStr">
+        <is>
+          <t>East Coast</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
@@ -2304,6 +2484,11 @@
           <t>DE</t>
         </is>
       </c>
+      <c r="O37" t="inlineStr">
+        <is>
+          <t>East Coast</t>
+        </is>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
@@ -2354,6 +2539,11 @@
           <t>MD</t>
         </is>
       </c>
+      <c r="O38" t="inlineStr">
+        <is>
+          <t>East Coast</t>
+        </is>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
@@ -2404,6 +2594,11 @@
           <t>MD</t>
         </is>
       </c>
+      <c r="O39" t="inlineStr">
+        <is>
+          <t>East Coast</t>
+        </is>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
@@ -2454,6 +2649,11 @@
           <t>MD</t>
         </is>
       </c>
+      <c r="O40" t="inlineStr">
+        <is>
+          <t>East Coast</t>
+        </is>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
@@ -2504,6 +2704,11 @@
           <t>MD</t>
         </is>
       </c>
+      <c r="O41" t="inlineStr">
+        <is>
+          <t>East Coast</t>
+        </is>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
@@ -2554,6 +2759,11 @@
           <t>MD</t>
         </is>
       </c>
+      <c r="O42" t="inlineStr">
+        <is>
+          <t>East Coast</t>
+        </is>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
@@ -2604,6 +2814,11 @@
           <t>MD</t>
         </is>
       </c>
+      <c r="O43" t="inlineStr">
+        <is>
+          <t>East Coast</t>
+        </is>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
@@ -2654,6 +2869,11 @@
           <t>MD</t>
         </is>
       </c>
+      <c r="O44" t="inlineStr">
+        <is>
+          <t>East Coast</t>
+        </is>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
@@ -2704,6 +2924,11 @@
           <t>DC</t>
         </is>
       </c>
+      <c r="O45" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
@@ -2754,6 +2979,11 @@
           <t>VA</t>
         </is>
       </c>
+      <c r="O46" t="inlineStr">
+        <is>
+          <t>East Coast</t>
+        </is>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
@@ -2804,6 +3034,11 @@
           <t>VA</t>
         </is>
       </c>
+      <c r="O47" t="inlineStr">
+        <is>
+          <t>East Coast</t>
+        </is>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
@@ -2854,6 +3089,11 @@
           <t>VA</t>
         </is>
       </c>
+      <c r="O48" t="inlineStr">
+        <is>
+          <t>East Coast</t>
+        </is>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
@@ -2904,6 +3144,11 @@
           <t>VA</t>
         </is>
       </c>
+      <c r="O49" t="inlineStr">
+        <is>
+          <t>East Coast</t>
+        </is>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
@@ -2954,6 +3199,11 @@
           <t>VA</t>
         </is>
       </c>
+      <c r="O50" t="inlineStr">
+        <is>
+          <t>East Coast</t>
+        </is>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
@@ -3004,6 +3254,11 @@
           <t>VA</t>
         </is>
       </c>
+      <c r="O51" t="inlineStr">
+        <is>
+          <t>East Coast</t>
+        </is>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
@@ -3054,6 +3309,11 @@
           <t>VA</t>
         </is>
       </c>
+      <c r="O52" t="inlineStr">
+        <is>
+          <t>East Coast</t>
+        </is>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
@@ -3104,6 +3364,11 @@
           <t>VA</t>
         </is>
       </c>
+      <c r="O53" t="inlineStr">
+        <is>
+          <t>East Coast</t>
+        </is>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
@@ -3154,6 +3419,11 @@
           <t>VA</t>
         </is>
       </c>
+      <c r="O54" t="inlineStr">
+        <is>
+          <t>East Coast</t>
+        </is>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
@@ -3204,6 +3474,11 @@
           <t>NC</t>
         </is>
       </c>
+      <c r="O55" t="inlineStr">
+        <is>
+          <t>East Coast</t>
+        </is>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
@@ -3254,6 +3529,11 @@
           <t>NC</t>
         </is>
       </c>
+      <c r="O56" t="inlineStr">
+        <is>
+          <t>East Coast</t>
+        </is>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
@@ -3304,6 +3584,11 @@
           <t>NC</t>
         </is>
       </c>
+      <c r="O57" t="inlineStr">
+        <is>
+          <t>East Coast</t>
+        </is>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
@@ -3354,6 +3639,11 @@
           <t>NC</t>
         </is>
       </c>
+      <c r="O58" t="inlineStr">
+        <is>
+          <t>East Coast</t>
+        </is>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
@@ -3404,6 +3694,11 @@
           <t>SC</t>
         </is>
       </c>
+      <c r="O59" t="inlineStr">
+        <is>
+          <t>East Coast</t>
+        </is>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
@@ -3454,6 +3749,11 @@
           <t>SC</t>
         </is>
       </c>
+      <c r="O60" t="inlineStr">
+        <is>
+          <t>East Coast</t>
+        </is>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
@@ -3504,6 +3804,11 @@
           <t>GA</t>
         </is>
       </c>
+      <c r="O61" t="inlineStr">
+        <is>
+          <t>East Coast</t>
+        </is>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="n">
@@ -3554,6 +3859,11 @@
           <t>FL</t>
         </is>
       </c>
+      <c r="O62" t="inlineStr">
+        <is>
+          <t>Gulf Coast</t>
+        </is>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="n">
@@ -3604,6 +3914,11 @@
           <t>FL</t>
         </is>
       </c>
+      <c r="O63" t="inlineStr">
+        <is>
+          <t>Gulf Coast</t>
+        </is>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="n">
@@ -3654,6 +3969,11 @@
           <t>FL</t>
         </is>
       </c>
+      <c r="O64" t="inlineStr">
+        <is>
+          <t>Gulf Coast</t>
+        </is>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="n">
@@ -3704,6 +4024,11 @@
           <t>FL</t>
         </is>
       </c>
+      <c r="O65" t="inlineStr">
+        <is>
+          <t>Gulf Coast</t>
+        </is>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="n">
@@ -3754,6 +4079,11 @@
           <t>FL</t>
         </is>
       </c>
+      <c r="O66" t="inlineStr">
+        <is>
+          <t>Gulf Coast</t>
+        </is>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="n">
@@ -3804,6 +4134,11 @@
           <t>FL</t>
         </is>
       </c>
+      <c r="O67" t="inlineStr">
+        <is>
+          <t>Gulf Coast</t>
+        </is>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="n">
@@ -3854,6 +4189,11 @@
           <t>FL</t>
         </is>
       </c>
+      <c r="O68" t="inlineStr">
+        <is>
+          <t>Gulf Coast</t>
+        </is>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="n">
@@ -3904,6 +4244,11 @@
           <t>FL</t>
         </is>
       </c>
+      <c r="O69" t="inlineStr">
+        <is>
+          <t>Gulf Coast</t>
+        </is>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="n">
@@ -3954,6 +4299,11 @@
           <t>FL</t>
         </is>
       </c>
+      <c r="O70" t="inlineStr">
+        <is>
+          <t>Gulf Coast</t>
+        </is>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="n">
@@ -4004,6 +4354,11 @@
           <t>FL</t>
         </is>
       </c>
+      <c r="O71" t="inlineStr">
+        <is>
+          <t>Gulf Coast</t>
+        </is>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="n">
@@ -4054,6 +4409,11 @@
           <t>FL</t>
         </is>
       </c>
+      <c r="O72" t="inlineStr">
+        <is>
+          <t>Gulf Coast</t>
+        </is>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="n">
@@ -4104,6 +4464,11 @@
           <t>FL</t>
         </is>
       </c>
+      <c r="O73" t="inlineStr">
+        <is>
+          <t>Gulf Coast</t>
+        </is>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="n">
@@ -4154,6 +4519,11 @@
           <t>FL</t>
         </is>
       </c>
+      <c r="O74" t="inlineStr">
+        <is>
+          <t>Gulf Coast</t>
+        </is>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="n">
@@ -4204,6 +4574,11 @@
           <t>FL</t>
         </is>
       </c>
+      <c r="O75" t="inlineStr">
+        <is>
+          <t>Gulf Coast</t>
+        </is>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="n">
@@ -4254,6 +4629,11 @@
           <t>FL</t>
         </is>
       </c>
+      <c r="O76" t="inlineStr">
+        <is>
+          <t>Gulf Coast</t>
+        </is>
+      </c>
     </row>
     <row r="77">
       <c r="A77" t="n">
@@ -4304,6 +4684,11 @@
           <t>FL</t>
         </is>
       </c>
+      <c r="O77" t="inlineStr">
+        <is>
+          <t>Gulf Coast</t>
+        </is>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="n">
@@ -4354,6 +4739,11 @@
           <t>FL</t>
         </is>
       </c>
+      <c r="O78" t="inlineStr">
+        <is>
+          <t>Gulf Coast</t>
+        </is>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="n">
@@ -4404,6 +4794,11 @@
           <t>FL</t>
         </is>
       </c>
+      <c r="O79" t="inlineStr">
+        <is>
+          <t>Gulf Coast</t>
+        </is>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="n">
@@ -4454,6 +4849,11 @@
           <t>AL</t>
         </is>
       </c>
+      <c r="O80" t="inlineStr">
+        <is>
+          <t>Gulf Coast</t>
+        </is>
+      </c>
     </row>
     <row r="81">
       <c r="A81" t="n">
@@ -4504,6 +4904,11 @@
           <t>AL</t>
         </is>
       </c>
+      <c r="O81" t="inlineStr">
+        <is>
+          <t>Gulf Coast</t>
+        </is>
+      </c>
     </row>
     <row r="82">
       <c r="A82" t="n">
@@ -4554,6 +4959,11 @@
           <t>MS</t>
         </is>
       </c>
+      <c r="O82" t="inlineStr">
+        <is>
+          <t>Gulf Coast</t>
+        </is>
+      </c>
     </row>
     <row r="83">
       <c r="A83" t="n">
@@ -4604,6 +5014,11 @@
           <t>LA</t>
         </is>
       </c>
+      <c r="O83" t="inlineStr">
+        <is>
+          <t>Gulf Coast</t>
+        </is>
+      </c>
     </row>
     <row r="84">
       <c r="A84" t="n">
@@ -4654,6 +5069,11 @@
           <t>LA</t>
         </is>
       </c>
+      <c r="O84" t="inlineStr">
+        <is>
+          <t>Gulf Coast</t>
+        </is>
+      </c>
     </row>
     <row r="85">
       <c r="A85" t="n">
@@ -4704,6 +5124,11 @@
           <t>TX</t>
         </is>
       </c>
+      <c r="O85" t="inlineStr">
+        <is>
+          <t>Gulf Coast</t>
+        </is>
+      </c>
     </row>
     <row r="86">
       <c r="A86" t="n">
@@ -4754,6 +5179,11 @@
           <t>TX</t>
         </is>
       </c>
+      <c r="O86" t="inlineStr">
+        <is>
+          <t>Gulf Coast</t>
+        </is>
+      </c>
     </row>
     <row r="87">
       <c r="A87" t="n">
@@ -4804,6 +5234,11 @@
           <t>TX</t>
         </is>
       </c>
+      <c r="O87" t="inlineStr">
+        <is>
+          <t>Gulf Coast</t>
+        </is>
+      </c>
     </row>
     <row r="88">
       <c r="A88" t="n">
@@ -4854,6 +5289,11 @@
           <t>TX</t>
         </is>
       </c>
+      <c r="O88" t="inlineStr">
+        <is>
+          <t>Gulf Coast</t>
+        </is>
+      </c>
     </row>
     <row r="89">
       <c r="A89" t="n">
@@ -4904,6 +5344,11 @@
           <t>TX</t>
         </is>
       </c>
+      <c r="O89" t="inlineStr">
+        <is>
+          <t>Gulf Coast</t>
+        </is>
+      </c>
     </row>
     <row r="90">
       <c r="A90" t="n">
@@ -4954,6 +5399,11 @@
           <t>TX</t>
         </is>
       </c>
+      <c r="O90" t="inlineStr">
+        <is>
+          <t>Gulf Coast</t>
+        </is>
+      </c>
     </row>
     <row r="91">
       <c r="A91" t="n">
@@ -5004,6 +5454,11 @@
           <t>TX</t>
         </is>
       </c>
+      <c r="O91" t="inlineStr">
+        <is>
+          <t>Gulf Coast</t>
+        </is>
+      </c>
     </row>
     <row r="92">
       <c r="A92" t="n">
@@ -5054,6 +5509,11 @@
           <t>TX</t>
         </is>
       </c>
+      <c r="O92" t="inlineStr">
+        <is>
+          <t>Gulf Coast</t>
+        </is>
+      </c>
     </row>
     <row r="93">
       <c r="A93" t="n">
@@ -5104,6 +5564,11 @@
           <t>TX</t>
         </is>
       </c>
+      <c r="O93" t="inlineStr">
+        <is>
+          <t>Gulf Coast</t>
+        </is>
+      </c>
     </row>
     <row r="94">
       <c r="A94" t="n">
@@ -5154,6 +5619,11 @@
           <t>TX</t>
         </is>
       </c>
+      <c r="O94" t="inlineStr">
+        <is>
+          <t>Gulf Coast</t>
+        </is>
+      </c>
     </row>
     <row r="95">
       <c r="A95" t="n">
@@ -5204,6 +5674,11 @@
           <t>TX</t>
         </is>
       </c>
+      <c r="O95" t="inlineStr">
+        <is>
+          <t>Gulf Coast</t>
+        </is>
+      </c>
     </row>
     <row r="96">
       <c r="A96" t="n">
@@ -5254,6 +5729,11 @@
           <t>TX</t>
         </is>
       </c>
+      <c r="O96" t="inlineStr">
+        <is>
+          <t>Gulf Coast</t>
+        </is>
+      </c>
     </row>
     <row r="97">
       <c r="A97" t="n">
@@ -5304,6 +5784,11 @@
           <t>TX</t>
         </is>
       </c>
+      <c r="O97" t="inlineStr">
+        <is>
+          <t>Gulf Coast</t>
+        </is>
+      </c>
     </row>
     <row r="98">
       <c r="A98" t="n">
@@ -5354,6 +5839,11 @@
           <t>CA</t>
         </is>
       </c>
+      <c r="O98" t="inlineStr">
+        <is>
+          <t>West Coast</t>
+        </is>
+      </c>
     </row>
     <row r="99">
       <c r="A99" t="n">
@@ -5404,6 +5894,11 @@
           <t>CA</t>
         </is>
       </c>
+      <c r="O99" t="inlineStr">
+        <is>
+          <t>West Coast</t>
+        </is>
+      </c>
     </row>
     <row r="100">
       <c r="A100" t="n">
@@ -5454,6 +5949,11 @@
           <t>CA</t>
         </is>
       </c>
+      <c r="O100" t="inlineStr">
+        <is>
+          <t>West Coast</t>
+        </is>
+      </c>
     </row>
     <row r="101">
       <c r="A101" t="n">
@@ -5504,6 +6004,11 @@
           <t>CA</t>
         </is>
       </c>
+      <c r="O101" t="inlineStr">
+        <is>
+          <t>West Coast</t>
+        </is>
+      </c>
     </row>
     <row r="102">
       <c r="A102" t="n">
@@ -5554,6 +6059,11 @@
           <t>CA</t>
         </is>
       </c>
+      <c r="O102" t="inlineStr">
+        <is>
+          <t>West Coast</t>
+        </is>
+      </c>
     </row>
     <row r="103">
       <c r="A103" t="n">
@@ -5604,6 +6114,11 @@
           <t>CA</t>
         </is>
       </c>
+      <c r="O103" t="inlineStr">
+        <is>
+          <t>West Coast</t>
+        </is>
+      </c>
     </row>
     <row r="104">
       <c r="A104" t="n">
@@ -5654,6 +6169,11 @@
           <t>CA</t>
         </is>
       </c>
+      <c r="O104" t="inlineStr">
+        <is>
+          <t>West Coast</t>
+        </is>
+      </c>
     </row>
     <row r="105">
       <c r="A105" t="n">
@@ -5704,6 +6224,11 @@
           <t>CA</t>
         </is>
       </c>
+      <c r="O105" t="inlineStr">
+        <is>
+          <t>West Coast</t>
+        </is>
+      </c>
     </row>
     <row r="106">
       <c r="A106" t="n">
@@ -5754,6 +6279,11 @@
           <t>CA</t>
         </is>
       </c>
+      <c r="O106" t="inlineStr">
+        <is>
+          <t>West Coast</t>
+        </is>
+      </c>
     </row>
     <row r="107">
       <c r="A107" t="n">
@@ -5804,6 +6334,11 @@
           <t>CA</t>
         </is>
       </c>
+      <c r="O107" t="inlineStr">
+        <is>
+          <t>West Coast</t>
+        </is>
+      </c>
     </row>
     <row r="108">
       <c r="A108" t="n">
@@ -5854,6 +6389,11 @@
           <t>CA</t>
         </is>
       </c>
+      <c r="O108" t="inlineStr">
+        <is>
+          <t>West Coast</t>
+        </is>
+      </c>
     </row>
     <row r="109">
       <c r="A109" t="n">
@@ -5904,6 +6444,11 @@
           <t>CA</t>
         </is>
       </c>
+      <c r="O109" t="inlineStr">
+        <is>
+          <t>West Coast</t>
+        </is>
+      </c>
     </row>
     <row r="110">
       <c r="A110" t="n">
@@ -5954,6 +6499,11 @@
           <t>CA</t>
         </is>
       </c>
+      <c r="O110" t="inlineStr">
+        <is>
+          <t>West Coast</t>
+        </is>
+      </c>
     </row>
     <row r="111">
       <c r="A111" t="n">
@@ -6004,6 +6554,11 @@
           <t>CA</t>
         </is>
       </c>
+      <c r="O111" t="inlineStr">
+        <is>
+          <t>West Coast</t>
+        </is>
+      </c>
     </row>
     <row r="112">
       <c r="A112" t="n">
@@ -6054,6 +6609,11 @@
           <t>CA</t>
         </is>
       </c>
+      <c r="O112" t="inlineStr">
+        <is>
+          <t>West Coast</t>
+        </is>
+      </c>
     </row>
     <row r="113">
       <c r="A113" t="n">
@@ -6104,6 +6664,11 @@
           <t>OR</t>
         </is>
       </c>
+      <c r="O113" t="inlineStr">
+        <is>
+          <t>West Coast</t>
+        </is>
+      </c>
     </row>
     <row r="114">
       <c r="A114" t="n">
@@ -6154,6 +6719,11 @@
           <t>OR</t>
         </is>
       </c>
+      <c r="O114" t="inlineStr">
+        <is>
+          <t>West Coast</t>
+        </is>
+      </c>
     </row>
     <row r="115">
       <c r="A115" t="n">
@@ -6204,6 +6774,11 @@
           <t>OR</t>
         </is>
       </c>
+      <c r="O115" t="inlineStr">
+        <is>
+          <t>West Coast</t>
+        </is>
+      </c>
     </row>
     <row r="116">
       <c r="A116" t="n">
@@ -6254,6 +6829,11 @@
           <t>OR</t>
         </is>
       </c>
+      <c r="O116" t="inlineStr">
+        <is>
+          <t>West Coast</t>
+        </is>
+      </c>
     </row>
     <row r="117">
       <c r="A117" t="n">
@@ -6304,6 +6884,11 @@
           <t>OR</t>
         </is>
       </c>
+      <c r="O117" t="inlineStr">
+        <is>
+          <t>West Coast</t>
+        </is>
+      </c>
     </row>
     <row r="118">
       <c r="A118" t="n">
@@ -6354,6 +6939,11 @@
           <t>WA</t>
         </is>
       </c>
+      <c r="O118" t="inlineStr">
+        <is>
+          <t>West Coast</t>
+        </is>
+      </c>
     </row>
     <row r="119">
       <c r="A119" t="n">
@@ -6404,6 +6994,11 @@
           <t>WA</t>
         </is>
       </c>
+      <c r="O119" t="inlineStr">
+        <is>
+          <t>West Coast</t>
+        </is>
+      </c>
     </row>
     <row r="120">
       <c r="A120" t="n">
@@ -6454,6 +7049,11 @@
           <t>WA</t>
         </is>
       </c>
+      <c r="O120" t="inlineStr">
+        <is>
+          <t>West Coast</t>
+        </is>
+      </c>
     </row>
     <row r="121">
       <c r="A121" t="n">
@@ -6504,6 +7104,11 @@
           <t>WA</t>
         </is>
       </c>
+      <c r="O121" t="inlineStr">
+        <is>
+          <t>West Coast</t>
+        </is>
+      </c>
     </row>
     <row r="122">
       <c r="A122" t="n">
@@ -6554,6 +7159,11 @@
           <t>WA</t>
         </is>
       </c>
+      <c r="O122" t="inlineStr">
+        <is>
+          <t>West Coast</t>
+        </is>
+      </c>
     </row>
     <row r="123">
       <c r="A123" t="n">
@@ -6604,6 +7214,11 @@
           <t>WA</t>
         </is>
       </c>
+      <c r="O123" t="inlineStr">
+        <is>
+          <t>West Coast</t>
+        </is>
+      </c>
     </row>
     <row r="124">
       <c r="A124" t="n">
@@ -6654,6 +7269,11 @@
           <t>WA</t>
         </is>
       </c>
+      <c r="O124" t="inlineStr">
+        <is>
+          <t>West Coast</t>
+        </is>
+      </c>
     </row>
     <row r="125">
       <c r="A125" t="n">
@@ -6704,6 +7324,11 @@
           <t>AK</t>
         </is>
       </c>
+      <c r="O125" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
     </row>
     <row r="126">
       <c r="A126" t="n">
@@ -6754,6 +7379,11 @@
           <t>AK</t>
         </is>
       </c>
+      <c r="O126" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
     </row>
     <row r="127">
       <c r="A127" t="n">
@@ -6804,6 +7434,11 @@
           <t>AK</t>
         </is>
       </c>
+      <c r="O127" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
     </row>
     <row r="128">
       <c r="A128" t="n">
@@ -6854,6 +7489,11 @@
           <t>AK</t>
         </is>
       </c>
+      <c r="O128" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
     </row>
     <row r="129">
       <c r="A129" t="n">
@@ -6904,6 +7544,11 @@
           <t>AK</t>
         </is>
       </c>
+      <c r="O129" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
     </row>
     <row r="130">
       <c r="A130" t="n">
@@ -6954,6 +7599,11 @@
           <t>AK</t>
         </is>
       </c>
+      <c r="O130" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
     </row>
     <row r="131">
       <c r="A131" t="n">
@@ -7004,6 +7654,11 @@
           <t>AK</t>
         </is>
       </c>
+      <c r="O131" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
     </row>
     <row r="132">
       <c r="A132" t="n">
@@ -7054,6 +7709,11 @@
           <t>AK</t>
         </is>
       </c>
+      <c r="O132" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
     </row>
     <row r="133">
       <c r="A133" t="n">
@@ -7104,6 +7764,11 @@
           <t>AK</t>
         </is>
       </c>
+      <c r="O133" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
     </row>
     <row r="134">
       <c r="A134" t="n">
@@ -7154,6 +7819,11 @@
           <t>AK</t>
         </is>
       </c>
+      <c r="O134" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
     </row>
     <row r="135">
       <c r="A135" t="n">
@@ -7204,6 +7874,11 @@
           <t>AK</t>
         </is>
       </c>
+      <c r="O135" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
     </row>
     <row r="136">
       <c r="A136" t="n">
@@ -7254,6 +7929,11 @@
           <t>AK</t>
         </is>
       </c>
+      <c r="O136" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
     </row>
     <row r="137">
       <c r="A137" t="n">
@@ -7304,6 +7984,11 @@
           <t>AK</t>
         </is>
       </c>
+      <c r="O137" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
     </row>
     <row r="138">
       <c r="A138" t="n">
@@ -7354,6 +8039,11 @@
           <t>AK</t>
         </is>
       </c>
+      <c r="O138" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
     </row>
     <row r="139">
       <c r="A139" t="n">
@@ -7404,6 +8094,11 @@
           <t>AK</t>
         </is>
       </c>
+      <c r="O139" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
     </row>
     <row r="140">
       <c r="A140" t="n">
@@ -7454,6 +8149,11 @@
           <t>AK</t>
         </is>
       </c>
+      <c r="O140" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
     </row>
     <row r="141">
       <c r="A141" t="n">
@@ -7504,6 +8204,11 @@
           <t>AK</t>
         </is>
       </c>
+      <c r="O141" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
     </row>
     <row r="142">
       <c r="A142" t="n">
@@ -7554,6 +8259,11 @@
           <t>AK</t>
         </is>
       </c>
+      <c r="O142" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
     </row>
     <row r="143">
       <c r="A143" t="n">
@@ -7604,6 +8314,11 @@
           <t>VI</t>
         </is>
       </c>
+      <c r="O143" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
     </row>
     <row r="144">
       <c r="A144" t="n">
@@ -7654,6 +8369,11 @@
           <t>VI</t>
         </is>
       </c>
+      <c r="O144" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
     </row>
     <row r="145">
       <c r="A145" t="n">
@@ -7704,6 +8424,11 @@
           <t>PR</t>
         </is>
       </c>
+      <c r="O145" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
     </row>
     <row r="146">
       <c r="A146" t="n">
@@ -7752,6 +8477,11 @@
       <c r="N146" t="inlineStr">
         <is>
           <t>PR</t>
+        </is>
+      </c>
+      <c r="O146" t="inlineStr">
+        <is>
+          <t>Other</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update dependencies and save beach data to Excel file
</commit_message>
<xml_diff>
--- a/data/usstations.xlsx
+++ b/data/usstations.xlsx
@@ -561,7 +561,7 @@
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>Island</t>
         </is>
       </c>
     </row>
@@ -616,7 +616,7 @@
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>Island</t>
         </is>
       </c>
     </row>
@@ -671,7 +671,7 @@
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>Island</t>
         </is>
       </c>
     </row>
@@ -726,7 +726,7 @@
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>Island</t>
         </is>
       </c>
     </row>
@@ -781,7 +781,7 @@
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>Island</t>
         </is>
       </c>
     </row>
@@ -836,7 +836,7 @@
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>Island</t>
         </is>
       </c>
     </row>
@@ -1056,7 +1056,7 @@
       </c>
       <c r="O11" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>Island</t>
         </is>
       </c>
     </row>
@@ -1111,7 +1111,7 @@
       </c>
       <c r="O12" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>Island</t>
         </is>
       </c>
     </row>
@@ -1166,7 +1166,7 @@
       </c>
       <c r="O13" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>Island</t>
         </is>
       </c>
     </row>
@@ -1221,7 +1221,7 @@
       </c>
       <c r="O14" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>Island</t>
         </is>
       </c>
     </row>
@@ -2376,7 +2376,7 @@
       </c>
       <c r="O35" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>East Coast</t>
         </is>
       </c>
     </row>
@@ -2926,7 +2926,7 @@
       </c>
       <c r="O45" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>East Coast</t>
         </is>
       </c>
     </row>
@@ -7326,7 +7326,7 @@
       </c>
       <c r="O125" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>West Coast</t>
         </is>
       </c>
     </row>
@@ -7381,7 +7381,7 @@
       </c>
       <c r="O126" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>West Coast</t>
         </is>
       </c>
     </row>
@@ -7436,7 +7436,7 @@
       </c>
       <c r="O127" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>West Coast</t>
         </is>
       </c>
     </row>
@@ -7491,7 +7491,7 @@
       </c>
       <c r="O128" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>West Coast</t>
         </is>
       </c>
     </row>
@@ -7546,7 +7546,7 @@
       </c>
       <c r="O129" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>West Coast</t>
         </is>
       </c>
     </row>
@@ -7601,7 +7601,7 @@
       </c>
       <c r="O130" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>West Coast</t>
         </is>
       </c>
     </row>
@@ -7656,7 +7656,7 @@
       </c>
       <c r="O131" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>West Coast</t>
         </is>
       </c>
     </row>
@@ -7711,7 +7711,7 @@
       </c>
       <c r="O132" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>West Coast</t>
         </is>
       </c>
     </row>
@@ -7766,7 +7766,7 @@
       </c>
       <c r="O133" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>West Coast</t>
         </is>
       </c>
     </row>
@@ -7821,7 +7821,7 @@
       </c>
       <c r="O134" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>West Coast</t>
         </is>
       </c>
     </row>
@@ -7876,7 +7876,7 @@
       </c>
       <c r="O135" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>West Coast</t>
         </is>
       </c>
     </row>
@@ -7931,7 +7931,7 @@
       </c>
       <c r="O136" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>West Coast</t>
         </is>
       </c>
     </row>
@@ -7986,7 +7986,7 @@
       </c>
       <c r="O137" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>West Coast</t>
         </is>
       </c>
     </row>
@@ -8041,7 +8041,7 @@
       </c>
       <c r="O138" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>West Coast</t>
         </is>
       </c>
     </row>
@@ -8096,7 +8096,7 @@
       </c>
       <c r="O139" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>West Coast</t>
         </is>
       </c>
     </row>
@@ -8151,7 +8151,7 @@
       </c>
       <c r="O140" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>West Coast</t>
         </is>
       </c>
     </row>
@@ -8206,7 +8206,7 @@
       </c>
       <c r="O141" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>West Coast</t>
         </is>
       </c>
     </row>
@@ -8261,7 +8261,7 @@
       </c>
       <c r="O142" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>West Coast</t>
         </is>
       </c>
     </row>
@@ -8426,7 +8426,7 @@
       </c>
       <c r="O145" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>Island</t>
         </is>
       </c>
     </row>
@@ -8481,7 +8481,7 @@
       </c>
       <c r="O146" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>Island</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update project overview and features
</commit_message>
<xml_diff>
--- a/data/usstations.xlsx
+++ b/data/usstations.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1056,7 +1056,7 @@
       </c>
       <c r="O11" t="inlineStr">
         <is>
-          <t>Island</t>
+          <t>Other</t>
         </is>
       </c>
     </row>

</xml_diff>